<commit_message>
Adding AggressiveCows.java and updating list
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1737,11 +1737,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B125" activeCellId="0" sqref="B125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3000,24 +3000,24 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="12" t="s">
+      <c r="A121" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B121" s="13" t="s">
+      <c r="B121" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C121" s="5" t="s">
+      <c r="C121" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="12" t="s">
+      <c r="A122" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B122" s="13" t="s">
+      <c r="B122" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="5" t="s">
+      <c r="C122" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3032,80 +3032,80 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="12" t="s">
+    <row r="124" customFormat="false" ht="20.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="B124" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C124" s="5" t="s">
+      <c r="C124" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="12" t="s">
+      <c r="A125" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B125" s="13" t="s">
+      <c r="B125" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C125" s="5" t="s">
+      <c r="C125" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="12" t="s">
+      <c r="A126" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B126" s="13" t="s">
+      <c r="B126" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C126" s="5" t="s">
+      <c r="C126" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="12" t="s">
+      <c r="A127" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B127" s="13" t="s">
+      <c r="B127" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C127" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="12" t="s">
+      <c r="A128" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B128" s="13" t="s">
+      <c r="B128" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="C128" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="12" t="s">
+      <c r="A129" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="C129" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="12" t="s">
+      <c r="A130" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B130" s="13" t="s">
+      <c r="B130" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C130" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Linked List questions and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1737,11 +1737,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B125" activeCellId="0" sqref="B125"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3110,24 +3110,24 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="12" t="s">
+      <c r="A131" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B131" s="13" t="s">
+      <c r="B131" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C131" s="5" t="s">
+      <c r="C131" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="12" t="s">
+      <c r="A132" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B132" s="13" t="s">
+      <c r="B132" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C132" s="5" t="s">
+      <c r="C132" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3143,35 +3143,35 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="12" t="s">
+      <c r="A134" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B134" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C134" s="5" t="s">
+      <c r="C134" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="12" t="s">
+      <c r="A135" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B135" s="13" t="s">
+      <c r="B135" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="C135" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="12" t="s">
+      <c r="A136" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C136" s="5" t="s">
+      <c r="C136" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3179,113 +3179,113 @@
       <c r="B138" s="17"/>
       <c r="C138" s="5"/>
     </row>
-    <row r="139" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="12" t="s">
+    <row r="139" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B139" s="13" t="s">
+      <c r="B139" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C139" s="5" t="s">
+      <c r="C139" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="12" t="s">
+      <c r="A140" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B140" s="13" t="s">
+      <c r="B140" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C140" s="5" t="s">
+      <c r="C140" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="12" t="s">
+      <c r="A141" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B141" s="13" t="s">
+      <c r="B141" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C141" s="5" t="s">
+      <c r="C141" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="12" t="s">
+      <c r="A142" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B142" s="13" t="s">
+      <c r="B142" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C142" s="5" t="s">
+      <c r="C142" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="12" t="s">
+      <c r="A143" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B143" s="13" t="s">
+      <c r="B143" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C143" s="5" t="s">
+      <c r="C143" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="12" t="s">
+      <c r="A144" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B144" s="13" t="s">
+      <c r="B144" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C144" s="5" t="s">
+      <c r="C144" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="12" t="s">
+      <c r="A145" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C145" s="5" t="s">
+      <c r="C145" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="12" t="s">
+      <c r="A146" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B146" s="13" t="s">
+      <c r="B146" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C146" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="12" t="s">
+      <c r="A147" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C147" s="5" t="s">
+      <c r="C147" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="12" t="s">
+      <c r="A148" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B148" s="13" t="s">
+      <c r="B148" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="C148" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding 2 more Linked list questions and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1737,11 +1737,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A139" activeCellId="0" sqref="A139"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A140" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B162" activeCellId="0" sqref="B162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3290,24 +3290,24 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="12" t="s">
+      <c r="A149" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B149" s="13" t="s">
+      <c r="B149" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C149" s="5" t="s">
+      <c r="C149" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="12" t="s">
+      <c r="A150" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B150" s="13" t="s">
+      <c r="B150" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C150" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3334,68 +3334,68 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="12" t="s">
+      <c r="A153" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B153" s="13" t="s">
+      <c r="B153" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C153" s="5" t="s">
+      <c r="C153" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="12" t="s">
+      <c r="A154" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B154" s="13" t="s">
+      <c r="B154" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C154" s="5" t="s">
+      <c r="C154" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="12" t="s">
+      <c r="A155" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B155" s="13" t="s">
+      <c r="B155" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C155" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="12" t="s">
+      <c r="A156" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B156" s="13" t="s">
+      <c r="B156" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C156" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="12" t="s">
+      <c r="A157" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B157" s="13" t="s">
+      <c r="B157" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C157" s="5" t="s">
+      <c r="C157" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="12" t="s">
+      <c r="A158" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B158" s="13" t="s">
+      <c r="B158" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C158" s="5" t="s">
+      <c r="C158" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding Binary Trees' first 10 questions and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="467">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t xml:space="preserve">Program for n’th node from the end of a Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Traversal ??</t>
   </si>
   <si>
     <t xml:space="preserve">Find the first non-repeating character from a stream of characters</t>
@@ -1568,7 +1571,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1651,6 +1654,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1737,15 +1744,16 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A140" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B162" activeCellId="0" sqref="B162"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A186" activeCellId="0" sqref="A186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3311,14 +3319,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="12" t="s">
+    <row r="151" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B151" s="13" t="s">
+      <c r="B151" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C151" s="5" t="s">
+      <c r="C151" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3400,79 +3408,79 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="12" t="s">
+      <c r="A159" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B159" s="13" t="s">
+      <c r="B159" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C159" s="5" t="s">
+      <c r="C159" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="12" t="s">
+      <c r="A160" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B160" s="13" t="s">
+      <c r="B160" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C160" s="5" t="s">
+      <c r="C160" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="12" t="s">
+      <c r="A161" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B161" s="13" t="s">
+      <c r="B161" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C161" s="5" t="s">
+      <c r="C161" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="12" t="s">
+      <c r="A162" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B162" s="13" t="s">
+      <c r="B162" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C162" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="12" t="s">
+      <c r="A163" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B163" s="13" t="s">
+      <c r="B163" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C163" s="5" t="s">
+      <c r="C163" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="12" t="s">
+      <c r="A164" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B164" s="17" t="s">
+      <c r="B164" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C164" s="5" t="s">
+      <c r="C164" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="12" t="s">
+      <c r="A165" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B165" s="17" t="s">
+      <c r="B165" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="C165" s="5" t="s">
+      <c r="C165" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3488,24 +3496,24 @@
       </c>
     </row>
     <row r="167" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="12" t="s">
+      <c r="A167" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B167" s="13" t="s">
+      <c r="B167" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C167" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="12" t="s">
+      <c r="C167" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B168" s="13" t="s">
+      <c r="B168" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C168" s="5" t="s">
+      <c r="C168" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3521,47 +3529,50 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="12" t="s">
+      <c r="A170" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B170" s="13" t="s">
+      <c r="B170" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C170" s="5" t="s">
+      <c r="C170" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="12" t="s">
+      <c r="A171" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B171" s="13" t="s">
+      <c r="B171" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C171" s="5" t="s">
+      <c r="C171" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="12" t="s">
+      <c r="A172" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B172" s="13" t="s">
+      <c r="B172" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C172" s="5" t="s">
+      <c r="C172" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="12" t="s">
+      <c r="A173" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B173" s="13" t="s">
+      <c r="B173" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C173" s="5" t="s">
-        <v>5</v>
+      <c r="C173" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,7 +3580,7 @@
         <v>136</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>5</v>
@@ -3580,121 +3591,121 @@
       <c r="C176" s="5"/>
     </row>
     <row r="177" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B177" s="13" t="s">
+      <c r="A177" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C177" s="5" t="s">
+      <c r="B177" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C177" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B178" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C178" s="5" t="s">
+      <c r="A178" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C178" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B179" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C179" s="5" t="s">
+      <c r="A179" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C179" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B180" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C180" s="5" t="s">
+      <c r="A180" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C180" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B181" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C181" s="5" t="s">
+      <c r="A181" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C181" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B182" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="C182" s="5" t="s">
+      <c r="A182" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C182" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B183" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C183" s="5" t="s">
+      <c r="A183" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C183" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B184" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C184" s="5" t="s">
+      <c r="A184" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C184" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B185" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C185" s="5" t="s">
+      <c r="A185" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C185" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B186" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C186" s="5" t="s">
+      <c r="A186" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C186" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>5</v>
@@ -3702,10 +3713,10 @@
     </row>
     <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C188" s="5" t="s">
         <v>5</v>
@@ -3713,10 +3724,10 @@
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C189" s="5" t="s">
         <v>5</v>
@@ -3724,10 +3735,10 @@
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>5</v>
@@ -3735,10 +3746,10 @@
     </row>
     <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C191" s="5" t="s">
         <v>5</v>
@@ -3746,10 +3757,10 @@
     </row>
     <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>5</v>
@@ -3757,10 +3768,10 @@
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>5</v>
@@ -3768,10 +3779,10 @@
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C194" s="5" t="s">
         <v>5</v>
@@ -3779,10 +3790,10 @@
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>5</v>
@@ -3790,10 +3801,10 @@
     </row>
     <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C196" s="5" t="s">
         <v>5</v>
@@ -3801,10 +3812,10 @@
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>5</v>
@@ -3812,10 +3823,10 @@
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>5</v>
@@ -3823,10 +3834,10 @@
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C199" s="5" t="s">
         <v>5</v>
@@ -3834,10 +3845,10 @@
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>5</v>
@@ -3845,10 +3856,10 @@
     </row>
     <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>5</v>
@@ -3856,10 +3867,10 @@
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>5</v>
@@ -3867,10 +3878,10 @@
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C203" s="5" t="s">
         <v>5</v>
@@ -3878,10 +3889,10 @@
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C204" s="5" t="s">
         <v>5</v>
@@ -3889,10 +3900,10 @@
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>5</v>
@@ -3900,10 +3911,10 @@
     </row>
     <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>5</v>
@@ -3911,10 +3922,10 @@
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>5</v>
@@ -3922,10 +3933,10 @@
     </row>
     <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>5</v>
@@ -3933,10 +3944,10 @@
     </row>
     <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>5</v>
@@ -3944,10 +3955,10 @@
     </row>
     <row r="210" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>5</v>
@@ -3955,10 +3966,10 @@
     </row>
     <row r="211" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>5</v>
@@ -3976,10 +3987,10 @@
     </row>
     <row r="214" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B214" s="13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C214" s="5" t="s">
         <v>5</v>
@@ -3987,10 +3998,10 @@
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B215" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C215" s="5" t="s">
         <v>5</v>
@@ -3998,10 +4009,10 @@
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B216" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C216" s="5" t="s">
         <v>5</v>
@@ -4009,10 +4020,10 @@
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C217" s="5" t="s">
         <v>5</v>
@@ -4020,10 +4031,10 @@
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C218" s="5" t="s">
         <v>5</v>
@@ -4031,10 +4042,10 @@
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C219" s="5" t="s">
         <v>5</v>
@@ -4042,10 +4053,10 @@
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="B220" s="21" t="s">
-        <v>216</v>
+        <v>210</v>
+      </c>
+      <c r="B220" s="22" t="s">
+        <v>217</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>5</v>
@@ -4053,10 +4064,10 @@
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C221" s="5" t="s">
         <v>5</v>
@@ -4064,10 +4075,10 @@
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C222" s="5" t="s">
         <v>5</v>
@@ -4075,10 +4086,10 @@
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>5</v>
@@ -4086,10 +4097,10 @@
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C224" s="5" t="s">
         <v>5</v>
@@ -4097,10 +4108,10 @@
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C225" s="5" t="s">
         <v>5</v>
@@ -4108,10 +4119,10 @@
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>5</v>
@@ -4119,10 +4130,10 @@
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B227" s="13" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C227" s="5" t="s">
         <v>5</v>
@@ -4130,10 +4141,10 @@
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C228" s="5" t="s">
         <v>5</v>
@@ -4141,10 +4152,10 @@
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C229" s="5" t="s">
         <v>5</v>
@@ -4152,10 +4163,10 @@
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C230" s="5" t="s">
         <v>5</v>
@@ -4163,10 +4174,10 @@
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C231" s="5" t="s">
         <v>5</v>
@@ -4174,10 +4185,10 @@
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>5</v>
@@ -4185,10 +4196,10 @@
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>5</v>
@@ -4196,10 +4207,10 @@
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C234" s="5" t="s">
         <v>5</v>
@@ -4207,10 +4218,10 @@
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C235" s="5" t="s">
         <v>5</v>
@@ -4226,10 +4237,10 @@
     </row>
     <row r="238" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>5</v>
@@ -4237,10 +4248,10 @@
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>5</v>
@@ -4248,10 +4259,10 @@
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>5</v>
@@ -4259,10 +4270,10 @@
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>5</v>
@@ -4270,10 +4281,10 @@
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>5</v>
@@ -4281,10 +4292,10 @@
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>5</v>
@@ -4292,10 +4303,10 @@
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>5</v>
@@ -4303,10 +4314,10 @@
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>5</v>
@@ -4314,10 +4325,10 @@
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>5</v>
@@ -4325,10 +4336,10 @@
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>5</v>
@@ -4336,10 +4347,10 @@
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C248" s="5" t="s">
         <v>5</v>
@@ -4347,10 +4358,10 @@
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C249" s="5" t="s">
         <v>5</v>
@@ -4358,10 +4369,10 @@
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>5</v>
@@ -4369,10 +4380,10 @@
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C251" s="5" t="s">
         <v>5</v>
@@ -4380,10 +4391,10 @@
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>5</v>
@@ -4391,10 +4402,10 @@
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>5</v>
@@ -4402,10 +4413,10 @@
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>5</v>
@@ -4413,10 +4424,10 @@
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>5</v>
@@ -4424,10 +4435,10 @@
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>5</v>
@@ -4435,10 +4446,10 @@
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C257" s="5" t="s">
         <v>5</v>
@@ -4446,10 +4457,10 @@
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C258" s="5" t="s">
         <v>5</v>
@@ -4457,10 +4468,10 @@
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C259" s="5" t="s">
         <v>5</v>
@@ -4468,10 +4479,10 @@
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>5</v>
@@ -4479,10 +4490,10 @@
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>5</v>
@@ -4490,10 +4501,10 @@
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B262" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C262" s="5" t="s">
         <v>5</v>
@@ -4501,10 +4512,10 @@
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B263" s="13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>5</v>
@@ -4512,10 +4523,10 @@
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B264" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>5</v>
@@ -4523,10 +4534,10 @@
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B265" s="13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>5</v>
@@ -4534,10 +4545,10 @@
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B266" s="13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>5</v>
@@ -4545,10 +4556,10 @@
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B267" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>5</v>
@@ -4556,10 +4567,10 @@
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>5</v>
@@ -4567,10 +4578,10 @@
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B269" s="13" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>5</v>
@@ -4578,10 +4589,10 @@
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>5</v>
@@ -4589,7 +4600,7 @@
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B271" s="13" t="s">
         <v>88</v>
@@ -4600,10 +4611,10 @@
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>5</v>
@@ -4619,10 +4630,10 @@
     </row>
     <row r="275" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B275" s="13" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>5</v>
@@ -4630,10 +4641,10 @@
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B276" s="13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>5</v>
@@ -4641,10 +4652,10 @@
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B277" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>5</v>
@@ -4652,10 +4663,10 @@
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>5</v>
@@ -4663,10 +4674,10 @@
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>5</v>
@@ -4674,10 +4685,10 @@
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B280" s="13" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>5</v>
@@ -4685,10 +4696,10 @@
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>5</v>
@@ -4696,10 +4707,10 @@
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C282" s="5" t="s">
         <v>5</v>
@@ -4707,10 +4718,10 @@
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C283" s="5" t="s">
         <v>5</v>
@@ -4718,10 +4729,10 @@
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>5</v>
@@ -4729,10 +4740,10 @@
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>5</v>
@@ -4740,10 +4751,10 @@
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C286" s="5" t="s">
         <v>5</v>
@@ -4751,10 +4762,10 @@
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>5</v>
@@ -4762,10 +4773,10 @@
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C288" s="5" t="s">
         <v>5</v>
@@ -4773,10 +4784,10 @@
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>5</v>
@@ -4784,10 +4795,10 @@
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B290" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>5</v>
@@ -4795,10 +4806,10 @@
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C291" s="5" t="s">
         <v>5</v>
@@ -4806,10 +4817,10 @@
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C292" s="5" t="s">
         <v>5</v>
@@ -4817,10 +4828,10 @@
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>5</v>
@@ -4836,10 +4847,10 @@
     </row>
     <row r="296" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>5</v>
@@ -4847,10 +4858,10 @@
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C297" s="5" t="s">
         <v>5</v>
@@ -4858,10 +4869,10 @@
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>5</v>
@@ -4869,10 +4880,10 @@
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>5</v>
@@ -4880,10 +4891,10 @@
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>5</v>
@@ -4891,10 +4902,10 @@
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C301" s="5" t="s">
         <v>5</v>
@@ -4902,10 +4913,10 @@
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>5</v>
@@ -4913,10 +4924,10 @@
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B303" s="13" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>5</v>
@@ -4924,10 +4935,10 @@
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>5</v>
@@ -4935,10 +4946,10 @@
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C305" s="5" t="s">
         <v>5</v>
@@ -4946,10 +4957,10 @@
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C306" s="5" t="s">
         <v>5</v>
@@ -4957,10 +4968,10 @@
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C307" s="5" t="s">
         <v>5</v>
@@ -4968,10 +4979,10 @@
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C308" s="5" t="s">
         <v>5</v>
@@ -4979,10 +4990,10 @@
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="B309" s="21" t="s">
-        <v>301</v>
+        <v>288</v>
+      </c>
+      <c r="B309" s="22" t="s">
+        <v>302</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>5</v>
@@ -4990,10 +5001,10 @@
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>5</v>
@@ -5001,10 +5012,10 @@
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C311" s="5" t="s">
         <v>5</v>
@@ -5012,10 +5023,10 @@
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C312" s="5" t="s">
         <v>5</v>
@@ -5023,10 +5034,10 @@
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>5</v>
@@ -5034,10 +5045,10 @@
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C314" s="5" t="s">
         <v>5</v>
@@ -5045,10 +5056,10 @@
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>5</v>
@@ -5056,10 +5067,10 @@
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C316" s="5" t="s">
         <v>5</v>
@@ -5067,10 +5078,10 @@
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C317" s="5" t="s">
         <v>5</v>
@@ -5078,10 +5089,10 @@
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>5</v>
@@ -5089,10 +5100,10 @@
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>5</v>
@@ -5100,10 +5111,10 @@
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C320" s="5" t="s">
         <v>5</v>
@@ -5111,10 +5122,10 @@
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C321" s="5" t="s">
         <v>5</v>
@@ -5122,10 +5133,10 @@
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C322" s="5" t="s">
         <v>5</v>
@@ -5133,10 +5144,10 @@
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C323" s="5" t="s">
         <v>5</v>
@@ -5144,10 +5155,10 @@
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C324" s="5" t="s">
         <v>5</v>
@@ -5155,10 +5166,10 @@
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C325" s="5" t="s">
         <v>5</v>
@@ -5166,10 +5177,10 @@
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C326" s="5" t="s">
         <v>5</v>
@@ -5177,10 +5188,10 @@
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C327" s="5" t="s">
         <v>5</v>
@@ -5188,10 +5199,10 @@
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C328" s="5" t="s">
         <v>5</v>
@@ -5199,10 +5210,10 @@
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>5</v>
@@ -5210,10 +5221,10 @@
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C330" s="5" t="s">
         <v>5</v>
@@ -5221,10 +5232,10 @@
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C331" s="5" t="s">
         <v>5</v>
@@ -5232,10 +5243,10 @@
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C332" s="5" t="s">
         <v>5</v>
@@ -5243,10 +5254,10 @@
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C333" s="5" t="s">
         <v>5</v>
@@ -5262,10 +5273,10 @@
     </row>
     <row r="336" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>5</v>
@@ -5273,10 +5284,10 @@
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>5</v>
@@ -5284,10 +5295,10 @@
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>5</v>
@@ -5295,10 +5306,10 @@
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>5</v>
@@ -5306,10 +5317,10 @@
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>5</v>
@@ -5317,10 +5328,10 @@
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>5</v>
@@ -5328,10 +5339,10 @@
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>5</v>
@@ -5339,10 +5350,10 @@
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C343" s="5" t="s">
         <v>5</v>
@@ -5350,10 +5361,10 @@
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="B344" s="21" t="s">
-        <v>335</v>
+        <v>327</v>
+      </c>
+      <c r="B344" s="22" t="s">
+        <v>336</v>
       </c>
       <c r="C344" s="5" t="s">
         <v>5</v>
@@ -5361,10 +5372,10 @@
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>5</v>
@@ -5372,10 +5383,10 @@
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>5</v>
@@ -5383,10 +5394,10 @@
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>5</v>
@@ -5394,10 +5405,10 @@
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>5</v>
@@ -5405,10 +5416,10 @@
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>5</v>
@@ -5416,10 +5427,10 @@
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C350" s="5" t="s">
         <v>5</v>
@@ -5427,10 +5438,10 @@
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>5</v>
@@ -5438,10 +5449,10 @@
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>5</v>
@@ -5449,10 +5460,10 @@
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="12" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C353" s="5" t="s">
         <v>5</v>
@@ -5468,10 +5479,10 @@
     </row>
     <row r="356" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>5</v>
@@ -5479,10 +5490,10 @@
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C357" s="5" t="s">
         <v>5</v>
@@ -5490,10 +5501,10 @@
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>5</v>
@@ -5501,10 +5512,10 @@
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>5</v>
@@ -5512,10 +5523,10 @@
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C360" s="5" t="s">
         <v>5</v>
@@ -5523,10 +5534,10 @@
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C361" s="5" t="s">
         <v>5</v>
@@ -5534,10 +5545,10 @@
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C362" s="5" t="s">
         <v>5</v>
@@ -5545,10 +5556,10 @@
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>5</v>
@@ -5556,10 +5567,10 @@
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>5</v>
@@ -5567,10 +5578,10 @@
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>5</v>
@@ -5578,10 +5589,10 @@
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C366" s="5" t="s">
         <v>5</v>
@@ -5589,10 +5600,10 @@
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C367" s="5" t="s">
         <v>5</v>
@@ -5600,10 +5611,10 @@
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C368" s="5" t="s">
         <v>5</v>
@@ -5611,10 +5622,10 @@
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C369" s="5" t="s">
         <v>5</v>
@@ -5622,10 +5633,10 @@
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>5</v>
@@ -5633,10 +5644,10 @@
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C371" s="5" t="s">
         <v>5</v>
@@ -5644,10 +5655,10 @@
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C372" s="5" t="s">
         <v>5</v>
@@ -5655,10 +5666,10 @@
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C373" s="5" t="s">
         <v>5</v>
@@ -5666,10 +5677,10 @@
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>5</v>
@@ -5677,10 +5688,10 @@
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C375" s="5" t="s">
         <v>5</v>
@@ -5688,10 +5699,10 @@
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C376" s="5" t="s">
         <v>5</v>
@@ -5699,10 +5710,10 @@
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C377" s="5" t="s">
         <v>5</v>
@@ -5710,10 +5721,10 @@
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>5</v>
@@ -5721,10 +5732,10 @@
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C379" s="5" t="s">
         <v>5</v>
@@ -5732,10 +5743,10 @@
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C380" s="5" t="s">
         <v>5</v>
@@ -5743,10 +5754,10 @@
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C381" s="5" t="s">
         <v>5</v>
@@ -5754,10 +5765,10 @@
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C382" s="5" t="s">
         <v>5</v>
@@ -5765,10 +5776,10 @@
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C383" s="5" t="s">
         <v>5</v>
@@ -5776,10 +5787,10 @@
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C384" s="5" t="s">
         <v>5</v>
@@ -5787,10 +5798,10 @@
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>5</v>
@@ -5798,10 +5809,10 @@
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>5</v>
@@ -5809,10 +5820,10 @@
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>5</v>
@@ -5820,10 +5831,10 @@
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>5</v>
@@ -5831,10 +5842,10 @@
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>5</v>
@@ -5842,10 +5853,10 @@
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>5</v>
@@ -5853,10 +5864,10 @@
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>5</v>
@@ -5864,10 +5875,10 @@
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>5</v>
@@ -5875,10 +5886,10 @@
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>5</v>
@@ -5886,10 +5897,10 @@
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>5</v>
@@ -5897,10 +5908,10 @@
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>5</v>
@@ -5908,10 +5919,10 @@
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>5</v>
@@ -5919,10 +5930,10 @@
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>5</v>
@@ -5930,10 +5941,10 @@
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>5</v>
@@ -5941,10 +5952,10 @@
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C399" s="5" t="s">
         <v>5</v>
@@ -5960,10 +5971,10 @@
     </row>
     <row r="402" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>5</v>
@@ -5971,10 +5982,10 @@
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C403" s="5" t="s">
         <v>5</v>
@@ -5982,10 +5993,10 @@
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C404" s="5" t="s">
         <v>5</v>
@@ -5993,7 +6004,7 @@
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B405" s="13" t="s">
         <v>90</v>
@@ -6004,10 +6015,10 @@
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C406" s="5" t="s">
         <v>5</v>
@@ -6015,10 +6026,10 @@
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="12" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C407" s="5" t="s">
         <v>5</v>
@@ -6034,10 +6045,10 @@
     </row>
     <row r="410" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C410" s="5" t="s">
         <v>5</v>
@@ -6045,10 +6056,10 @@
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C411" s="5" t="s">
         <v>5</v>
@@ -6056,10 +6067,10 @@
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C412" s="5" t="s">
         <v>5</v>
@@ -6067,10 +6078,10 @@
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C413" s="5" t="s">
         <v>5</v>
@@ -6078,10 +6089,10 @@
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C414" s="5" t="s">
         <v>5</v>
@@ -6089,10 +6100,10 @@
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>5</v>
@@ -6100,10 +6111,10 @@
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C416" s="5" t="s">
         <v>5</v>
@@ -6111,10 +6122,10 @@
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C417" s="5" t="s">
         <v>5</v>
@@ -6122,10 +6133,10 @@
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C418" s="5" t="s">
         <v>5</v>
@@ -6133,10 +6144,10 @@
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C419" s="5" t="s">
         <v>5</v>
@@ -6144,10 +6155,10 @@
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C420" s="5" t="s">
         <v>5</v>
@@ -6155,10 +6166,10 @@
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C421" s="5" t="s">
         <v>5</v>
@@ -6166,10 +6177,10 @@
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>5</v>
@@ -6177,10 +6188,10 @@
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C423" s="5" t="s">
         <v>5</v>
@@ -6188,10 +6199,10 @@
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C424" s="5" t="s">
         <v>5</v>
@@ -6199,10 +6210,10 @@
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C425" s="5" t="s">
         <v>5</v>
@@ -6210,10 +6221,10 @@
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C426" s="5" t="s">
         <v>5</v>
@@ -6221,10 +6232,10 @@
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C427" s="5" t="s">
         <v>5</v>
@@ -6232,10 +6243,10 @@
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C428" s="5" t="s">
         <v>5</v>
@@ -6243,10 +6254,10 @@
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>5</v>
@@ -6254,10 +6265,10 @@
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>5</v>
@@ -6265,10 +6276,10 @@
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C431" s="5" t="s">
         <v>5</v>
@@ -6276,10 +6287,10 @@
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C432" s="5" t="s">
         <v>5</v>
@@ -6287,10 +6298,10 @@
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C433" s="5" t="s">
         <v>5</v>
@@ -6298,10 +6309,10 @@
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C434" s="5" t="s">
         <v>5</v>
@@ -6309,10 +6320,10 @@
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C435" s="5" t="s">
         <v>5</v>
@@ -6320,10 +6331,10 @@
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C436" s="5" t="s">
         <v>5</v>
@@ -6331,10 +6342,10 @@
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>5</v>
@@ -6342,10 +6353,10 @@
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C438" s="5" t="s">
         <v>5</v>
@@ -6353,10 +6364,10 @@
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>5</v>
@@ -6364,10 +6375,10 @@
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C440" s="5" t="s">
         <v>5</v>
@@ -6375,10 +6386,10 @@
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C441" s="5" t="s">
         <v>5</v>
@@ -6386,10 +6397,10 @@
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>5</v>
@@ -6397,10 +6408,10 @@
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>5</v>
@@ -6408,10 +6419,10 @@
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>5</v>
@@ -6419,10 +6430,10 @@
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>5</v>
@@ -6430,10 +6441,10 @@
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>5</v>
@@ -6441,10 +6452,10 @@
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C447" s="5" t="s">
         <v>5</v>
@@ -6452,10 +6463,10 @@
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>5</v>
@@ -6463,10 +6474,10 @@
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C449" s="5" t="s">
         <v>5</v>
@@ -6474,10 +6485,10 @@
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C450" s="5" t="s">
         <v>5</v>
@@ -6485,10 +6496,10 @@
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>5</v>
@@ -6496,10 +6507,10 @@
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>5</v>
@@ -6507,10 +6518,10 @@
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>5</v>
@@ -6518,10 +6529,10 @@
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>5</v>
@@ -6529,10 +6540,10 @@
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C455" s="5" t="s">
         <v>5</v>
@@ -6540,10 +6551,10 @@
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C456" s="5" t="s">
         <v>5</v>
@@ -6551,10 +6562,10 @@
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C457" s="5" t="s">
         <v>5</v>
@@ -6562,10 +6573,10 @@
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C458" s="5" t="s">
         <v>5</v>
@@ -6573,10 +6584,10 @@
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C459" s="5" t="s">
         <v>5</v>
@@ -6584,10 +6595,10 @@
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>5</v>
@@ -6595,10 +6606,10 @@
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>5</v>
@@ -6606,10 +6617,10 @@
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>5</v>
@@ -6617,10 +6628,10 @@
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>5</v>
@@ -6628,10 +6639,10 @@
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>5</v>
@@ -6639,10 +6650,10 @@
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C465" s="5" t="s">
         <v>5</v>
@@ -6650,10 +6661,10 @@
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>5</v>
@@ -6661,10 +6672,10 @@
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C467" s="5" t="s">
         <v>5</v>
@@ -6672,10 +6683,10 @@
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>5</v>
@@ -6683,10 +6694,10 @@
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C469" s="5" t="s">
         <v>5</v>
@@ -6703,10 +6714,10 @@
     </row>
     <row r="472" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>5</v>
@@ -6714,10 +6725,10 @@
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C473" s="5" t="s">
         <v>5</v>
@@ -6725,10 +6736,10 @@
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C474" s="5" t="s">
         <v>5</v>
@@ -6736,10 +6747,10 @@
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C475" s="5" t="s">
         <v>5</v>
@@ -6747,10 +6758,10 @@
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C476" s="5" t="s">
         <v>5</v>
@@ -6758,10 +6769,10 @@
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>5</v>
@@ -6769,10 +6780,10 @@
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>5</v>
@@ -6780,10 +6791,10 @@
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>5</v>
@@ -6791,10 +6802,10 @@
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>5</v>
@@ -6802,10 +6813,10 @@
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B481" s="13" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C481" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Adding 11-20 questions of Binary Trees, Min & Max Height of Binary Tree and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1502,7 +1502,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1531,6 +1531,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFE6E905"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3FAF46"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1571,7 +1577,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1660,6 +1666,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1725,7 +1743,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF3FAF46"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF224B12"/>
       <rgbColor rgb="FF993300"/>
@@ -1744,11 +1762,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A186" activeCellId="0" sqref="A186"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A197" activeCellId="0" sqref="A197"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3701,112 +3719,112 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="12" t="s">
+      <c r="A187" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B187" s="13" t="s">
+      <c r="B187" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C187" s="5" t="s">
+      <c r="C187" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="12" t="s">
+      <c r="A188" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B188" s="13" t="s">
+      <c r="B188" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="5" t="s">
+      <c r="C188" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="12" t="s">
+      <c r="A189" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B189" s="13" t="s">
+      <c r="B189" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="C189" s="5" t="s">
+      <c r="C189" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="12" t="s">
+      <c r="A190" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B190" s="13" t="s">
+      <c r="B190" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C190" s="5" t="s">
+      <c r="C190" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="12" t="s">
+      <c r="A191" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B191" s="13" t="s">
+      <c r="B191" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C191" s="5" t="s">
+      <c r="C191" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="12" t="s">
+      <c r="A192" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="B192" s="13" t="s">
+      <c r="B192" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="5" t="s">
+      <c r="C192" s="24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="12" t="s">
+      <c r="A193" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B193" s="13" t="s">
+      <c r="B193" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C193" s="5" t="s">
+      <c r="C193" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="12" t="s">
+      <c r="A194" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B194" s="13" t="s">
+      <c r="B194" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C194" s="5" t="s">
+      <c r="C194" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="12" t="s">
+      <c r="A195" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B195" s="13" t="s">
+      <c r="B195" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C195" s="5" t="s">
+      <c r="C195" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="12" t="s">
+      <c r="A196" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B196" s="13" t="s">
+      <c r="B196" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C196" s="5" t="s">
+      <c r="C196" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4055,7 +4073,7 @@
       <c r="A220" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="B220" s="22" t="s">
+      <c r="B220" s="25" t="s">
         <v>217</v>
       </c>
       <c r="C220" s="5" t="s">
@@ -4992,7 +5010,7 @@
       <c r="A309" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="B309" s="22" t="s">
+      <c r="B309" s="25" t="s">
         <v>302</v>
       </c>
       <c r="C309" s="5" t="s">
@@ -5363,7 +5381,7 @@
       <c r="A344" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="B344" s="22" t="s">
+      <c r="B344" s="25" t="s">
         <v>336</v>
       </c>
       <c r="C344" s="5" t="s">

</xml_diff>

<commit_message>
Adding next 10 questions of Binary Tree and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="468">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t xml:space="preserve">Check if all leaf nodes are at same level or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
   </si>
   <si>
     <t xml:space="preserve">Check if a Binary Tree contains duplicate subtrees of size 2 or more [ IMP ]</t>
@@ -1763,10 +1766,10 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A197" activeCellId="0" sqref="A197"/>
+      <selection pane="topLeft" activeCell="B194" activeCellId="0" sqref="B194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3829,46 +3832,46 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="12" t="s">
+      <c r="A197" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B197" s="13" t="s">
+      <c r="B197" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C197" s="5" t="s">
+      <c r="C197" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="12" t="s">
+      <c r="A198" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B198" s="13" t="s">
+      <c r="B198" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C198" s="5" t="s">
+      <c r="C198" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="12" t="s">
+      <c r="A199" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B199" s="13" t="s">
+      <c r="B199" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C199" s="5" t="s">
+      <c r="C199" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B200" s="13" t="s">
+      <c r="A200" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C200" s="5" t="s">
+      <c r="B200" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C200" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3877,64 +3880,64 @@
         <v>174</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="12" t="s">
+      <c r="A202" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B202" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C202" s="5" t="s">
+      <c r="B202" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C202" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="12" t="s">
+      <c r="A203" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="B203" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="C203" s="5" t="s">
+      <c r="B203" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C203" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="12" t="s">
+      <c r="A204" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B204" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C204" s="5" t="s">
+      <c r="B204" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C204" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="12" t="s">
+      <c r="A205" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B205" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C205" s="5" t="s">
+      <c r="B205" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C205" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="12" t="s">
+      <c r="A206" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B206" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C206" s="5" t="s">
+      <c r="B206" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C206" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3943,7 +3946,7 @@
         <v>174</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>5</v>
@@ -3954,7 +3957,7 @@
         <v>174</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>5</v>
@@ -3965,7 +3968,7 @@
         <v>174</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>5</v>
@@ -3976,7 +3979,7 @@
         <v>174</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>5</v>
@@ -3987,7 +3990,7 @@
         <v>174</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>5</v>
@@ -4005,10 +4008,10 @@
     </row>
     <row r="214" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B214" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C214" s="5" t="s">
         <v>5</v>
@@ -4016,10 +4019,10 @@
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B215" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C215" s="5" t="s">
         <v>5</v>
@@ -4027,10 +4030,10 @@
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B216" s="13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C216" s="5" t="s">
         <v>5</v>
@@ -4038,10 +4041,10 @@
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C217" s="5" t="s">
         <v>5</v>
@@ -4049,10 +4052,10 @@
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C218" s="5" t="s">
         <v>5</v>
@@ -4060,10 +4063,10 @@
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C219" s="5" t="s">
         <v>5</v>
@@ -4071,10 +4074,10 @@
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B220" s="25" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>5</v>
@@ -4082,10 +4085,10 @@
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C221" s="5" t="s">
         <v>5</v>
@@ -4093,10 +4096,10 @@
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C222" s="5" t="s">
         <v>5</v>
@@ -4104,10 +4107,10 @@
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>5</v>
@@ -4115,10 +4118,10 @@
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C224" s="5" t="s">
         <v>5</v>
@@ -4126,10 +4129,10 @@
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C225" s="5" t="s">
         <v>5</v>
@@ -4137,10 +4140,10 @@
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>5</v>
@@ -4148,10 +4151,10 @@
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B227" s="13" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C227" s="5" t="s">
         <v>5</v>
@@ -4159,10 +4162,10 @@
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C228" s="5" t="s">
         <v>5</v>
@@ -4170,10 +4173,10 @@
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C229" s="5" t="s">
         <v>5</v>
@@ -4181,10 +4184,10 @@
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C230" s="5" t="s">
         <v>5</v>
@@ -4192,10 +4195,10 @@
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C231" s="5" t="s">
         <v>5</v>
@@ -4203,10 +4206,10 @@
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>5</v>
@@ -4214,10 +4217,10 @@
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>5</v>
@@ -4225,10 +4228,10 @@
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C234" s="5" t="s">
         <v>5</v>
@@ -4236,10 +4239,10 @@
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C235" s="5" t="s">
         <v>5</v>
@@ -4255,10 +4258,10 @@
     </row>
     <row r="238" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>5</v>
@@ -4266,10 +4269,10 @@
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>5</v>
@@ -4277,10 +4280,10 @@
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>5</v>
@@ -4288,10 +4291,10 @@
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>5</v>
@@ -4299,10 +4302,10 @@
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>5</v>
@@ -4310,10 +4313,10 @@
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>5</v>
@@ -4321,10 +4324,10 @@
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>5</v>
@@ -4332,10 +4335,10 @@
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>5</v>
@@ -4343,10 +4346,10 @@
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>5</v>
@@ -4354,10 +4357,10 @@
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>5</v>
@@ -4365,10 +4368,10 @@
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C248" s="5" t="s">
         <v>5</v>
@@ -4376,10 +4379,10 @@
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C249" s="5" t="s">
         <v>5</v>
@@ -4387,10 +4390,10 @@
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>5</v>
@@ -4398,10 +4401,10 @@
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C251" s="5" t="s">
         <v>5</v>
@@ -4409,10 +4412,10 @@
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>5</v>
@@ -4420,10 +4423,10 @@
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>5</v>
@@ -4431,10 +4434,10 @@
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>5</v>
@@ -4442,10 +4445,10 @@
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>5</v>
@@ -4453,10 +4456,10 @@
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>5</v>
@@ -4464,10 +4467,10 @@
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C257" s="5" t="s">
         <v>5</v>
@@ -4475,10 +4478,10 @@
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C258" s="5" t="s">
         <v>5</v>
@@ -4486,10 +4489,10 @@
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C259" s="5" t="s">
         <v>5</v>
@@ -4497,10 +4500,10 @@
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>5</v>
@@ -4508,10 +4511,10 @@
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>5</v>
@@ -4519,10 +4522,10 @@
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B262" s="13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C262" s="5" t="s">
         <v>5</v>
@@ -4530,10 +4533,10 @@
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B263" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>5</v>
@@ -4541,10 +4544,10 @@
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B264" s="13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>5</v>
@@ -4552,10 +4555,10 @@
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B265" s="13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>5</v>
@@ -4563,10 +4566,10 @@
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B266" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>5</v>
@@ -4574,10 +4577,10 @@
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B267" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>5</v>
@@ -4585,10 +4588,10 @@
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>5</v>
@@ -4596,10 +4599,10 @@
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B269" s="13" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>5</v>
@@ -4607,10 +4610,10 @@
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>5</v>
@@ -4618,7 +4621,7 @@
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B271" s="13" t="s">
         <v>88</v>
@@ -4629,10 +4632,10 @@
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>5</v>
@@ -4648,10 +4651,10 @@
     </row>
     <row r="275" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B275" s="13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>5</v>
@@ -4659,10 +4662,10 @@
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B276" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>5</v>
@@ -4670,10 +4673,10 @@
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B277" s="13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>5</v>
@@ -4681,10 +4684,10 @@
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>5</v>
@@ -4692,10 +4695,10 @@
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>5</v>
@@ -4703,10 +4706,10 @@
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B280" s="13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>5</v>
@@ -4714,10 +4717,10 @@
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>5</v>
@@ -4725,10 +4728,10 @@
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C282" s="5" t="s">
         <v>5</v>
@@ -4736,10 +4739,10 @@
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C283" s="5" t="s">
         <v>5</v>
@@ -4747,10 +4750,10 @@
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>5</v>
@@ -4758,10 +4761,10 @@
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>5</v>
@@ -4769,10 +4772,10 @@
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C286" s="5" t="s">
         <v>5</v>
@@ -4780,10 +4783,10 @@
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>5</v>
@@ -4791,10 +4794,10 @@
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C288" s="5" t="s">
         <v>5</v>
@@ -4802,10 +4805,10 @@
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>5</v>
@@ -4813,10 +4816,10 @@
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B290" s="13" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>5</v>
@@ -4824,10 +4827,10 @@
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C291" s="5" t="s">
         <v>5</v>
@@ -4835,10 +4838,10 @@
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C292" s="5" t="s">
         <v>5</v>
@@ -4846,10 +4849,10 @@
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>5</v>
@@ -4865,10 +4868,10 @@
     </row>
     <row r="296" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>5</v>
@@ -4876,10 +4879,10 @@
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C297" s="5" t="s">
         <v>5</v>
@@ -4887,10 +4890,10 @@
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>5</v>
@@ -4898,10 +4901,10 @@
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>5</v>
@@ -4909,10 +4912,10 @@
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>5</v>
@@ -4920,10 +4923,10 @@
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C301" s="5" t="s">
         <v>5</v>
@@ -4931,10 +4934,10 @@
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>5</v>
@@ -4942,10 +4945,10 @@
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B303" s="13" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>5</v>
@@ -4953,10 +4956,10 @@
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>5</v>
@@ -4964,10 +4967,10 @@
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C305" s="5" t="s">
         <v>5</v>
@@ -4975,10 +4978,10 @@
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C306" s="5" t="s">
         <v>5</v>
@@ -4986,10 +4989,10 @@
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C307" s="5" t="s">
         <v>5</v>
@@ -4997,10 +5000,10 @@
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C308" s="5" t="s">
         <v>5</v>
@@ -5008,10 +5011,10 @@
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B309" s="25" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>5</v>
@@ -5019,10 +5022,10 @@
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>5</v>
@@ -5030,10 +5033,10 @@
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C311" s="5" t="s">
         <v>5</v>
@@ -5041,10 +5044,10 @@
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C312" s="5" t="s">
         <v>5</v>
@@ -5052,10 +5055,10 @@
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>5</v>
@@ -5063,10 +5066,10 @@
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C314" s="5" t="s">
         <v>5</v>
@@ -5074,10 +5077,10 @@
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>5</v>
@@ -5085,10 +5088,10 @@
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C316" s="5" t="s">
         <v>5</v>
@@ -5096,10 +5099,10 @@
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C317" s="5" t="s">
         <v>5</v>
@@ -5107,10 +5110,10 @@
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>5</v>
@@ -5118,10 +5121,10 @@
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>5</v>
@@ -5129,10 +5132,10 @@
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C320" s="5" t="s">
         <v>5</v>
@@ -5140,10 +5143,10 @@
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C321" s="5" t="s">
         <v>5</v>
@@ -5151,10 +5154,10 @@
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C322" s="5" t="s">
         <v>5</v>
@@ -5162,10 +5165,10 @@
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C323" s="5" t="s">
         <v>5</v>
@@ -5173,10 +5176,10 @@
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C324" s="5" t="s">
         <v>5</v>
@@ -5184,10 +5187,10 @@
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C325" s="5" t="s">
         <v>5</v>
@@ -5195,10 +5198,10 @@
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C326" s="5" t="s">
         <v>5</v>
@@ -5206,10 +5209,10 @@
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C327" s="5" t="s">
         <v>5</v>
@@ -5217,10 +5220,10 @@
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C328" s="5" t="s">
         <v>5</v>
@@ -5228,10 +5231,10 @@
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>5</v>
@@ -5239,10 +5242,10 @@
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C330" s="5" t="s">
         <v>5</v>
@@ -5250,10 +5253,10 @@
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C331" s="5" t="s">
         <v>5</v>
@@ -5261,10 +5264,10 @@
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C332" s="5" t="s">
         <v>5</v>
@@ -5272,10 +5275,10 @@
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C333" s="5" t="s">
         <v>5</v>
@@ -5291,10 +5294,10 @@
     </row>
     <row r="336" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>5</v>
@@ -5302,10 +5305,10 @@
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>5</v>
@@ -5313,10 +5316,10 @@
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>5</v>
@@ -5324,10 +5327,10 @@
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>5</v>
@@ -5335,10 +5338,10 @@
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>5</v>
@@ -5346,10 +5349,10 @@
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>5</v>
@@ -5357,10 +5360,10 @@
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>5</v>
@@ -5368,10 +5371,10 @@
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C343" s="5" t="s">
         <v>5</v>
@@ -5379,10 +5382,10 @@
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B344" s="25" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C344" s="5" t="s">
         <v>5</v>
@@ -5390,10 +5393,10 @@
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>5</v>
@@ -5401,10 +5404,10 @@
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>5</v>
@@ -5412,10 +5415,10 @@
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>5</v>
@@ -5423,10 +5426,10 @@
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>5</v>
@@ -5434,10 +5437,10 @@
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>5</v>
@@ -5445,10 +5448,10 @@
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C350" s="5" t="s">
         <v>5</v>
@@ -5456,10 +5459,10 @@
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>5</v>
@@ -5467,10 +5470,10 @@
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>5</v>
@@ -5478,10 +5481,10 @@
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C353" s="5" t="s">
         <v>5</v>
@@ -5497,10 +5500,10 @@
     </row>
     <row r="356" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>5</v>
@@ -5508,10 +5511,10 @@
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C357" s="5" t="s">
         <v>5</v>
@@ -5519,10 +5522,10 @@
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>5</v>
@@ -5530,10 +5533,10 @@
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>5</v>
@@ -5541,10 +5544,10 @@
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C360" s="5" t="s">
         <v>5</v>
@@ -5552,10 +5555,10 @@
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C361" s="5" t="s">
         <v>5</v>
@@ -5563,10 +5566,10 @@
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C362" s="5" t="s">
         <v>5</v>
@@ -5574,10 +5577,10 @@
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>5</v>
@@ -5585,10 +5588,10 @@
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>5</v>
@@ -5596,10 +5599,10 @@
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>5</v>
@@ -5607,10 +5610,10 @@
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C366" s="5" t="s">
         <v>5</v>
@@ -5618,10 +5621,10 @@
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C367" s="5" t="s">
         <v>5</v>
@@ -5629,10 +5632,10 @@
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C368" s="5" t="s">
         <v>5</v>
@@ -5640,10 +5643,10 @@
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C369" s="5" t="s">
         <v>5</v>
@@ -5651,10 +5654,10 @@
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>5</v>
@@ -5662,10 +5665,10 @@
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C371" s="5" t="s">
         <v>5</v>
@@ -5673,10 +5676,10 @@
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C372" s="5" t="s">
         <v>5</v>
@@ -5684,10 +5687,10 @@
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C373" s="5" t="s">
         <v>5</v>
@@ -5695,10 +5698,10 @@
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>5</v>
@@ -5706,10 +5709,10 @@
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C375" s="5" t="s">
         <v>5</v>
@@ -5717,10 +5720,10 @@
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C376" s="5" t="s">
         <v>5</v>
@@ -5728,10 +5731,10 @@
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C377" s="5" t="s">
         <v>5</v>
@@ -5739,10 +5742,10 @@
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>5</v>
@@ -5750,10 +5753,10 @@
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C379" s="5" t="s">
         <v>5</v>
@@ -5761,10 +5764,10 @@
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C380" s="5" t="s">
         <v>5</v>
@@ -5772,10 +5775,10 @@
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C381" s="5" t="s">
         <v>5</v>
@@ -5783,10 +5786,10 @@
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C382" s="5" t="s">
         <v>5</v>
@@ -5794,10 +5797,10 @@
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C383" s="5" t="s">
         <v>5</v>
@@ -5805,10 +5808,10 @@
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C384" s="5" t="s">
         <v>5</v>
@@ -5816,10 +5819,10 @@
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>5</v>
@@ -5827,10 +5830,10 @@
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>5</v>
@@ -5838,10 +5841,10 @@
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>5</v>
@@ -5849,10 +5852,10 @@
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>5</v>
@@ -5860,10 +5863,10 @@
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>5</v>
@@ -5871,10 +5874,10 @@
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>5</v>
@@ -5882,10 +5885,10 @@
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>5</v>
@@ -5893,10 +5896,10 @@
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>5</v>
@@ -5904,10 +5907,10 @@
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>5</v>
@@ -5915,10 +5918,10 @@
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>5</v>
@@ -5926,10 +5929,10 @@
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>5</v>
@@ -5937,10 +5940,10 @@
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>5</v>
@@ -5948,10 +5951,10 @@
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>5</v>
@@ -5959,10 +5962,10 @@
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>5</v>
@@ -5970,10 +5973,10 @@
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C399" s="5" t="s">
         <v>5</v>
@@ -5989,10 +5992,10 @@
     </row>
     <row r="402" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>5</v>
@@ -6000,10 +6003,10 @@
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C403" s="5" t="s">
         <v>5</v>
@@ -6011,10 +6014,10 @@
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C404" s="5" t="s">
         <v>5</v>
@@ -6022,7 +6025,7 @@
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B405" s="13" t="s">
         <v>90</v>
@@ -6033,10 +6036,10 @@
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C406" s="5" t="s">
         <v>5</v>
@@ -6044,10 +6047,10 @@
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C407" s="5" t="s">
         <v>5</v>
@@ -6063,10 +6066,10 @@
     </row>
     <row r="410" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C410" s="5" t="s">
         <v>5</v>
@@ -6074,10 +6077,10 @@
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C411" s="5" t="s">
         <v>5</v>
@@ -6085,10 +6088,10 @@
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C412" s="5" t="s">
         <v>5</v>
@@ -6096,10 +6099,10 @@
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C413" s="5" t="s">
         <v>5</v>
@@ -6107,10 +6110,10 @@
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C414" s="5" t="s">
         <v>5</v>
@@ -6118,10 +6121,10 @@
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>5</v>
@@ -6129,10 +6132,10 @@
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C416" s="5" t="s">
         <v>5</v>
@@ -6140,10 +6143,10 @@
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C417" s="5" t="s">
         <v>5</v>
@@ -6151,10 +6154,10 @@
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C418" s="5" t="s">
         <v>5</v>
@@ -6162,10 +6165,10 @@
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C419" s="5" t="s">
         <v>5</v>
@@ -6173,10 +6176,10 @@
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C420" s="5" t="s">
         <v>5</v>
@@ -6184,10 +6187,10 @@
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C421" s="5" t="s">
         <v>5</v>
@@ -6195,10 +6198,10 @@
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>5</v>
@@ -6206,10 +6209,10 @@
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C423" s="5" t="s">
         <v>5</v>
@@ -6217,10 +6220,10 @@
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C424" s="5" t="s">
         <v>5</v>
@@ -6228,10 +6231,10 @@
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C425" s="5" t="s">
         <v>5</v>
@@ -6239,10 +6242,10 @@
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C426" s="5" t="s">
         <v>5</v>
@@ -6250,10 +6253,10 @@
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C427" s="5" t="s">
         <v>5</v>
@@ -6261,10 +6264,10 @@
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C428" s="5" t="s">
         <v>5</v>
@@ -6272,10 +6275,10 @@
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>5</v>
@@ -6283,10 +6286,10 @@
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>5</v>
@@ -6294,10 +6297,10 @@
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C431" s="5" t="s">
         <v>5</v>
@@ -6305,10 +6308,10 @@
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C432" s="5" t="s">
         <v>5</v>
@@ -6316,10 +6319,10 @@
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C433" s="5" t="s">
         <v>5</v>
@@ -6327,10 +6330,10 @@
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C434" s="5" t="s">
         <v>5</v>
@@ -6338,10 +6341,10 @@
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C435" s="5" t="s">
         <v>5</v>
@@ -6349,10 +6352,10 @@
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C436" s="5" t="s">
         <v>5</v>
@@ -6360,10 +6363,10 @@
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>5</v>
@@ -6371,10 +6374,10 @@
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C438" s="5" t="s">
         <v>5</v>
@@ -6382,10 +6385,10 @@
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>5</v>
@@ -6393,10 +6396,10 @@
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C440" s="5" t="s">
         <v>5</v>
@@ -6404,10 +6407,10 @@
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C441" s="5" t="s">
         <v>5</v>
@@ -6415,10 +6418,10 @@
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>5</v>
@@ -6426,10 +6429,10 @@
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>5</v>
@@ -6437,10 +6440,10 @@
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>5</v>
@@ -6448,10 +6451,10 @@
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>5</v>
@@ -6459,10 +6462,10 @@
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>5</v>
@@ -6470,10 +6473,10 @@
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C447" s="5" t="s">
         <v>5</v>
@@ -6481,10 +6484,10 @@
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>5</v>
@@ -6492,10 +6495,10 @@
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C449" s="5" t="s">
         <v>5</v>
@@ -6503,10 +6506,10 @@
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C450" s="5" t="s">
         <v>5</v>
@@ -6514,10 +6517,10 @@
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>5</v>
@@ -6525,10 +6528,10 @@
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>5</v>
@@ -6536,10 +6539,10 @@
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>5</v>
@@ -6547,10 +6550,10 @@
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>5</v>
@@ -6558,10 +6561,10 @@
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C455" s="5" t="s">
         <v>5</v>
@@ -6569,10 +6572,10 @@
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C456" s="5" t="s">
         <v>5</v>
@@ -6580,10 +6583,10 @@
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C457" s="5" t="s">
         <v>5</v>
@@ -6591,10 +6594,10 @@
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C458" s="5" t="s">
         <v>5</v>
@@ -6602,10 +6605,10 @@
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C459" s="5" t="s">
         <v>5</v>
@@ -6613,10 +6616,10 @@
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>5</v>
@@ -6624,10 +6627,10 @@
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>5</v>
@@ -6635,10 +6638,10 @@
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>5</v>
@@ -6646,10 +6649,10 @@
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>5</v>
@@ -6657,10 +6660,10 @@
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>5</v>
@@ -6668,10 +6671,10 @@
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C465" s="5" t="s">
         <v>5</v>
@@ -6679,10 +6682,10 @@
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>5</v>
@@ -6690,10 +6693,10 @@
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C467" s="5" t="s">
         <v>5</v>
@@ -6701,10 +6704,10 @@
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>5</v>
@@ -6712,10 +6715,10 @@
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="12" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C469" s="5" t="s">
         <v>5</v>
@@ -6732,10 +6735,10 @@
     </row>
     <row r="472" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>5</v>
@@ -6743,10 +6746,10 @@
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C473" s="5" t="s">
         <v>5</v>
@@ -6754,10 +6757,10 @@
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C474" s="5" t="s">
         <v>5</v>
@@ -6765,10 +6768,10 @@
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C475" s="5" t="s">
         <v>5</v>
@@ -6776,10 +6779,10 @@
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C476" s="5" t="s">
         <v>5</v>
@@ -6787,10 +6790,10 @@
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>5</v>
@@ -6798,10 +6801,10 @@
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>5</v>
@@ -6809,10 +6812,10 @@
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>5</v>
@@ -6820,10 +6823,10 @@
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>5</v>
@@ -6831,10 +6834,10 @@
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="12" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B481" s="13" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C481" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Adding next 5 questions of Binary Trees and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1765,11 +1765,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B194" activeCellId="0" sqref="B194"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A207" activeCellId="0" sqref="A207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3942,57 +3942,57 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="12" t="s">
+      <c r="A207" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B207" s="13" t="s">
+      <c r="B207" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C207" s="5" t="s">
+      <c r="C207" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="12" t="s">
+      <c r="A208" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B208" s="13" t="s">
+      <c r="B208" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C208" s="5" t="s">
+      <c r="C208" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="12" t="s">
+      <c r="A209" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B209" s="13" t="s">
+      <c r="B209" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C209" s="5" t="s">
+      <c r="C209" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="12" t="s">
+      <c r="A210" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B210" s="13" t="s">
+      <c r="B210" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C210" s="5" t="s">
+      <c r="C210" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="12" t="s">
+      <c r="A211" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B211" s="13" t="s">
+      <c r="B211" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C211" s="5" t="s">
+      <c r="C211" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding BST questions and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1765,11 +1765,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A207" activeCellId="0" sqref="A207"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A206" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A217" activeCellId="0" sqref="A217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3791,7 +3791,7 @@
       <c r="A193" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B193" s="7" t="s">
+      <c r="B193" s="23" t="s">
         <v>191</v>
       </c>
       <c r="C193" s="8" t="s">
@@ -3824,7 +3824,7 @@
       <c r="A196" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B196" s="7" t="s">
+      <c r="B196" s="23" t="s">
         <v>194</v>
       </c>
       <c r="C196" s="8" t="s">

</xml_diff>

<commit_message>
Adding next 5 questions of BST and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="472">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t xml:space="preserve">Find Kth largest element in a BST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to do it in constant space</t>
   </si>
   <si>
     <t xml:space="preserve">Find Kth smallest element in a BST</t>
@@ -1778,11 +1781,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A212" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A229" activeCellId="0" sqref="A229"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A223" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A228" activeCellId="0" sqref="A228"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -4139,134 +4142,140 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="12" t="s">
+      <c r="A224" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B224" s="13" t="s">
+      <c r="B224" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C224" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="12" t="s">
+      <c r="C224" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B225" s="13" t="s">
+      <c r="B225" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C225" s="5" t="s">
-        <v>5</v>
+      <c r="C225" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D225" s="0" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="12" t="s">
+      <c r="A226" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B226" s="13" t="s">
+      <c r="B226" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C226" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D226" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="C226" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="12" t="s">
+      <c r="A227" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B227" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="C227" s="5" t="s">
+      <c r="B227" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C227" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="12" t="s">
+      <c r="A228" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B228" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C228" s="5" t="s">
+      <c r="B228" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C228" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="12" t="s">
+      <c r="A229" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B229" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C229" s="5" t="s">
+      <c r="B229" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C229" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="12" t="s">
+      <c r="A230" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B230" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C230" s="5" t="s">
+      <c r="B230" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C230" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="12" t="s">
+      <c r="A231" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B231" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C231" s="5" t="s">
+      <c r="B231" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C231" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="12" t="s">
+      <c r="A232" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B232" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="C232" s="5" t="s">
+      <c r="B232" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C232" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="12" t="s">
+      <c r="A233" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B233" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C233" s="5" t="s">
+      <c r="B233" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C233" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="12" t="s">
+      <c r="A234" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B234" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C234" s="5" t="s">
+      <c r="B234" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C234" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="12" t="s">
+      <c r="A235" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B235" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="C235" s="5" t="s">
+      <c r="B235" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C235" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4280,10 +4289,10 @@
     </row>
     <row r="238" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>5</v>
@@ -4291,10 +4300,10 @@
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>5</v>
@@ -4302,10 +4311,10 @@
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>5</v>
@@ -4313,10 +4322,10 @@
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>5</v>
@@ -4324,10 +4333,10 @@
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>5</v>
@@ -4335,10 +4344,10 @@
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>5</v>
@@ -4346,10 +4355,10 @@
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>5</v>
@@ -4357,10 +4366,10 @@
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>5</v>
@@ -4368,10 +4377,10 @@
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>5</v>
@@ -4379,10 +4388,10 @@
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>5</v>
@@ -4390,10 +4399,10 @@
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C248" s="5" t="s">
         <v>5</v>
@@ -4401,10 +4410,10 @@
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C249" s="5" t="s">
         <v>5</v>
@@ -4412,10 +4421,10 @@
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>5</v>
@@ -4423,10 +4432,10 @@
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C251" s="5" t="s">
         <v>5</v>
@@ -4434,10 +4443,10 @@
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>5</v>
@@ -4445,10 +4454,10 @@
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>5</v>
@@ -4456,10 +4465,10 @@
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>5</v>
@@ -4467,10 +4476,10 @@
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>5</v>
@@ -4478,10 +4487,10 @@
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>5</v>
@@ -4489,10 +4498,10 @@
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C257" s="5" t="s">
         <v>5</v>
@@ -4500,10 +4509,10 @@
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C258" s="5" t="s">
         <v>5</v>
@@ -4511,10 +4520,10 @@
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C259" s="5" t="s">
         <v>5</v>
@@ -4522,10 +4531,10 @@
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>5</v>
@@ -4533,10 +4542,10 @@
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>5</v>
@@ -4544,10 +4553,10 @@
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B262" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C262" s="5" t="s">
         <v>5</v>
@@ -4555,10 +4564,10 @@
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B263" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>5</v>
@@ -4566,10 +4575,10 @@
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B264" s="13" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>5</v>
@@ -4577,10 +4586,10 @@
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B265" s="13" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>5</v>
@@ -4588,10 +4597,10 @@
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B266" s="13" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>5</v>
@@ -4599,10 +4608,10 @@
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B267" s="13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>5</v>
@@ -4610,10 +4619,10 @@
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>5</v>
@@ -4621,10 +4630,10 @@
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B269" s="13" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>5</v>
@@ -4632,10 +4641,10 @@
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>5</v>
@@ -4643,7 +4652,7 @@
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B271" s="13" t="s">
         <v>88</v>
@@ -4654,10 +4663,10 @@
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>5</v>
@@ -4673,10 +4682,10 @@
     </row>
     <row r="275" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B275" s="13" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>5</v>
@@ -4684,10 +4693,10 @@
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B276" s="13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>5</v>
@@ -4695,10 +4704,10 @@
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B277" s="13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>5</v>
@@ -4706,10 +4715,10 @@
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>5</v>
@@ -4717,10 +4726,10 @@
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>5</v>
@@ -4728,10 +4737,10 @@
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B280" s="13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>5</v>
@@ -4739,10 +4748,10 @@
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>5</v>
@@ -4750,10 +4759,10 @@
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C282" s="5" t="s">
         <v>5</v>
@@ -4761,10 +4770,10 @@
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C283" s="5" t="s">
         <v>5</v>
@@ -4772,10 +4781,10 @@
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>5</v>
@@ -4783,10 +4792,10 @@
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>5</v>
@@ -4794,10 +4803,10 @@
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C286" s="5" t="s">
         <v>5</v>
@@ -4805,10 +4814,10 @@
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>5</v>
@@ -4816,10 +4825,10 @@
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C288" s="5" t="s">
         <v>5</v>
@@ -4827,10 +4836,10 @@
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>5</v>
@@ -4838,10 +4847,10 @@
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B290" s="13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>5</v>
@@ -4849,10 +4858,10 @@
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C291" s="5" t="s">
         <v>5</v>
@@ -4860,10 +4869,10 @@
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C292" s="5" t="s">
         <v>5</v>
@@ -4871,10 +4880,10 @@
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>5</v>
@@ -4890,10 +4899,10 @@
     </row>
     <row r="296" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>5</v>
@@ -4901,10 +4910,10 @@
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C297" s="5" t="s">
         <v>5</v>
@@ -4912,10 +4921,10 @@
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>5</v>
@@ -4923,10 +4932,10 @@
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>5</v>
@@ -4934,10 +4943,10 @@
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>5</v>
@@ -4945,10 +4954,10 @@
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C301" s="5" t="s">
         <v>5</v>
@@ -4956,10 +4965,10 @@
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>5</v>
@@ -4967,10 +4976,10 @@
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B303" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>5</v>
@@ -4978,10 +4987,10 @@
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>5</v>
@@ -4989,10 +4998,10 @@
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C305" s="5" t="s">
         <v>5</v>
@@ -5000,10 +5009,10 @@
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C306" s="5" t="s">
         <v>5</v>
@@ -5011,10 +5020,10 @@
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C307" s="5" t="s">
         <v>5</v>
@@ -5022,10 +5031,10 @@
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C308" s="5" t="s">
         <v>5</v>
@@ -5033,10 +5042,10 @@
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B309" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>5</v>
@@ -5044,10 +5053,10 @@
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>5</v>
@@ -5055,10 +5064,10 @@
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C311" s="5" t="s">
         <v>5</v>
@@ -5066,10 +5075,10 @@
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C312" s="5" t="s">
         <v>5</v>
@@ -5077,10 +5086,10 @@
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>5</v>
@@ -5088,10 +5097,10 @@
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C314" s="5" t="s">
         <v>5</v>
@@ -5099,10 +5108,10 @@
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>5</v>
@@ -5110,10 +5119,10 @@
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C316" s="5" t="s">
         <v>5</v>
@@ -5121,10 +5130,10 @@
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C317" s="5" t="s">
         <v>5</v>
@@ -5132,10 +5141,10 @@
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>5</v>
@@ -5143,10 +5152,10 @@
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>5</v>
@@ -5154,10 +5163,10 @@
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C320" s="5" t="s">
         <v>5</v>
@@ -5165,10 +5174,10 @@
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C321" s="5" t="s">
         <v>5</v>
@@ -5176,10 +5185,10 @@
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C322" s="5" t="s">
         <v>5</v>
@@ -5187,10 +5196,10 @@
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C323" s="5" t="s">
         <v>5</v>
@@ -5198,10 +5207,10 @@
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C324" s="5" t="s">
         <v>5</v>
@@ -5209,10 +5218,10 @@
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C325" s="5" t="s">
         <v>5</v>
@@ -5220,10 +5229,10 @@
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C326" s="5" t="s">
         <v>5</v>
@@ -5231,10 +5240,10 @@
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C327" s="5" t="s">
         <v>5</v>
@@ -5242,10 +5251,10 @@
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C328" s="5" t="s">
         <v>5</v>
@@ -5253,10 +5262,10 @@
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>5</v>
@@ -5264,10 +5273,10 @@
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C330" s="5" t="s">
         <v>5</v>
@@ -5275,10 +5284,10 @@
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C331" s="5" t="s">
         <v>5</v>
@@ -5286,10 +5295,10 @@
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C332" s="5" t="s">
         <v>5</v>
@@ -5297,10 +5306,10 @@
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C333" s="5" t="s">
         <v>5</v>
@@ -5316,10 +5325,10 @@
     </row>
     <row r="336" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>5</v>
@@ -5327,10 +5336,10 @@
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>5</v>
@@ -5338,10 +5347,10 @@
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>5</v>
@@ -5349,10 +5358,10 @@
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>5</v>
@@ -5360,10 +5369,10 @@
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>5</v>
@@ -5371,10 +5380,10 @@
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>5</v>
@@ -5382,10 +5391,10 @@
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>5</v>
@@ -5393,10 +5402,10 @@
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C343" s="5" t="s">
         <v>5</v>
@@ -5404,10 +5413,10 @@
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B344" s="26" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C344" s="5" t="s">
         <v>5</v>
@@ -5415,10 +5424,10 @@
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>5</v>
@@ -5426,10 +5435,10 @@
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>5</v>
@@ -5437,10 +5446,10 @@
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>5</v>
@@ -5448,10 +5457,10 @@
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>5</v>
@@ -5459,10 +5468,10 @@
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>5</v>
@@ -5470,10 +5479,10 @@
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C350" s="5" t="s">
         <v>5</v>
@@ -5481,10 +5490,10 @@
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>5</v>
@@ -5492,10 +5501,10 @@
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>5</v>
@@ -5503,10 +5512,10 @@
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C353" s="5" t="s">
         <v>5</v>
@@ -5522,10 +5531,10 @@
     </row>
     <row r="356" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>5</v>
@@ -5533,10 +5542,10 @@
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C357" s="5" t="s">
         <v>5</v>
@@ -5544,10 +5553,10 @@
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>5</v>
@@ -5555,10 +5564,10 @@
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>5</v>
@@ -5566,10 +5575,10 @@
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C360" s="5" t="s">
         <v>5</v>
@@ -5577,10 +5586,10 @@
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C361" s="5" t="s">
         <v>5</v>
@@ -5588,10 +5597,10 @@
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C362" s="5" t="s">
         <v>5</v>
@@ -5599,10 +5608,10 @@
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>5</v>
@@ -5610,10 +5619,10 @@
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>5</v>
@@ -5621,10 +5630,10 @@
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>5</v>
@@ -5632,10 +5641,10 @@
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C366" s="5" t="s">
         <v>5</v>
@@ -5643,10 +5652,10 @@
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C367" s="5" t="s">
         <v>5</v>
@@ -5654,10 +5663,10 @@
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C368" s="5" t="s">
         <v>5</v>
@@ -5665,10 +5674,10 @@
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C369" s="5" t="s">
         <v>5</v>
@@ -5676,10 +5685,10 @@
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>5</v>
@@ -5687,10 +5696,10 @@
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C371" s="5" t="s">
         <v>5</v>
@@ -5698,10 +5707,10 @@
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C372" s="5" t="s">
         <v>5</v>
@@ -5709,10 +5718,10 @@
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C373" s="5" t="s">
         <v>5</v>
@@ -5720,10 +5729,10 @@
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>5</v>
@@ -5731,10 +5740,10 @@
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C375" s="5" t="s">
         <v>5</v>
@@ -5742,10 +5751,10 @@
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C376" s="5" t="s">
         <v>5</v>
@@ -5753,10 +5762,10 @@
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C377" s="5" t="s">
         <v>5</v>
@@ -5764,10 +5773,10 @@
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>5</v>
@@ -5775,10 +5784,10 @@
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C379" s="5" t="s">
         <v>5</v>
@@ -5786,10 +5795,10 @@
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C380" s="5" t="s">
         <v>5</v>
@@ -5797,10 +5806,10 @@
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C381" s="5" t="s">
         <v>5</v>
@@ -5808,10 +5817,10 @@
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C382" s="5" t="s">
         <v>5</v>
@@ -5819,10 +5828,10 @@
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C383" s="5" t="s">
         <v>5</v>
@@ -5830,10 +5839,10 @@
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C384" s="5" t="s">
         <v>5</v>
@@ -5841,10 +5850,10 @@
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>5</v>
@@ -5852,10 +5861,10 @@
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>5</v>
@@ -5863,10 +5872,10 @@
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>5</v>
@@ -5874,10 +5883,10 @@
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>5</v>
@@ -5885,10 +5894,10 @@
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>5</v>
@@ -5896,10 +5905,10 @@
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>5</v>
@@ -5907,10 +5916,10 @@
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>5</v>
@@ -5918,10 +5927,10 @@
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>5</v>
@@ -5929,10 +5938,10 @@
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>5</v>
@@ -5940,10 +5949,10 @@
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>5</v>
@@ -5951,10 +5960,10 @@
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>5</v>
@@ -5962,10 +5971,10 @@
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>5</v>
@@ -5973,10 +5982,10 @@
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>5</v>
@@ -5984,10 +5993,10 @@
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>5</v>
@@ -5995,10 +6004,10 @@
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C399" s="5" t="s">
         <v>5</v>
@@ -6014,10 +6023,10 @@
     </row>
     <row r="402" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>5</v>
@@ -6025,10 +6034,10 @@
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C403" s="5" t="s">
         <v>5</v>
@@ -6036,10 +6045,10 @@
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C404" s="5" t="s">
         <v>5</v>
@@ -6047,7 +6056,7 @@
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B405" s="13" t="s">
         <v>90</v>
@@ -6058,10 +6067,10 @@
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C406" s="5" t="s">
         <v>5</v>
@@ -6069,10 +6078,10 @@
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C407" s="5" t="s">
         <v>5</v>
@@ -6088,10 +6097,10 @@
     </row>
     <row r="410" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C410" s="5" t="s">
         <v>5</v>
@@ -6099,10 +6108,10 @@
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C411" s="5" t="s">
         <v>5</v>
@@ -6110,10 +6119,10 @@
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C412" s="5" t="s">
         <v>5</v>
@@ -6121,10 +6130,10 @@
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C413" s="5" t="s">
         <v>5</v>
@@ -6132,10 +6141,10 @@
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C414" s="5" t="s">
         <v>5</v>
@@ -6143,10 +6152,10 @@
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>5</v>
@@ -6154,10 +6163,10 @@
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C416" s="5" t="s">
         <v>5</v>
@@ -6165,10 +6174,10 @@
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C417" s="5" t="s">
         <v>5</v>
@@ -6176,10 +6185,10 @@
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C418" s="5" t="s">
         <v>5</v>
@@ -6187,10 +6196,10 @@
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C419" s="5" t="s">
         <v>5</v>
@@ -6198,10 +6207,10 @@
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C420" s="5" t="s">
         <v>5</v>
@@ -6209,10 +6218,10 @@
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C421" s="5" t="s">
         <v>5</v>
@@ -6220,10 +6229,10 @@
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>5</v>
@@ -6231,10 +6240,10 @@
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C423" s="5" t="s">
         <v>5</v>
@@ -6242,10 +6251,10 @@
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C424" s="5" t="s">
         <v>5</v>
@@ -6253,10 +6262,10 @@
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C425" s="5" t="s">
         <v>5</v>
@@ -6264,10 +6273,10 @@
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C426" s="5" t="s">
         <v>5</v>
@@ -6275,10 +6284,10 @@
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C427" s="5" t="s">
         <v>5</v>
@@ -6286,10 +6295,10 @@
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C428" s="5" t="s">
         <v>5</v>
@@ -6297,10 +6306,10 @@
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>5</v>
@@ -6308,10 +6317,10 @@
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>5</v>
@@ -6319,10 +6328,10 @@
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C431" s="5" t="s">
         <v>5</v>
@@ -6330,10 +6339,10 @@
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C432" s="5" t="s">
         <v>5</v>
@@ -6341,10 +6350,10 @@
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C433" s="5" t="s">
         <v>5</v>
@@ -6352,10 +6361,10 @@
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C434" s="5" t="s">
         <v>5</v>
@@ -6363,10 +6372,10 @@
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C435" s="5" t="s">
         <v>5</v>
@@ -6374,10 +6383,10 @@
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C436" s="5" t="s">
         <v>5</v>
@@ -6385,10 +6394,10 @@
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>5</v>
@@ -6396,10 +6405,10 @@
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C438" s="5" t="s">
         <v>5</v>
@@ -6407,10 +6416,10 @@
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>5</v>
@@ -6418,10 +6427,10 @@
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C440" s="5" t="s">
         <v>5</v>
@@ -6429,10 +6438,10 @@
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C441" s="5" t="s">
         <v>5</v>
@@ -6440,10 +6449,10 @@
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>5</v>
@@ -6451,10 +6460,10 @@
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>5</v>
@@ -6462,10 +6471,10 @@
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>5</v>
@@ -6473,10 +6482,10 @@
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>5</v>
@@ -6484,10 +6493,10 @@
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>5</v>
@@ -6495,10 +6504,10 @@
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C447" s="5" t="s">
         <v>5</v>
@@ -6506,10 +6515,10 @@
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>5</v>
@@ -6517,10 +6526,10 @@
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C449" s="5" t="s">
         <v>5</v>
@@ -6528,10 +6537,10 @@
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C450" s="5" t="s">
         <v>5</v>
@@ -6539,10 +6548,10 @@
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>5</v>
@@ -6550,10 +6559,10 @@
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>5</v>
@@ -6561,10 +6570,10 @@
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>5</v>
@@ -6572,10 +6581,10 @@
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>5</v>
@@ -6583,10 +6592,10 @@
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C455" s="5" t="s">
         <v>5</v>
@@ -6594,10 +6603,10 @@
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C456" s="5" t="s">
         <v>5</v>
@@ -6605,10 +6614,10 @@
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C457" s="5" t="s">
         <v>5</v>
@@ -6616,10 +6625,10 @@
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C458" s="5" t="s">
         <v>5</v>
@@ -6627,10 +6636,10 @@
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C459" s="5" t="s">
         <v>5</v>
@@ -6638,10 +6647,10 @@
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>5</v>
@@ -6649,10 +6658,10 @@
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>5</v>
@@ -6660,10 +6669,10 @@
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>5</v>
@@ -6671,10 +6680,10 @@
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>5</v>
@@ -6682,10 +6691,10 @@
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>5</v>
@@ -6693,10 +6702,10 @@
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C465" s="5" t="s">
         <v>5</v>
@@ -6704,10 +6713,10 @@
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>5</v>
@@ -6715,10 +6724,10 @@
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C467" s="5" t="s">
         <v>5</v>
@@ -6726,10 +6735,10 @@
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>5</v>
@@ -6737,10 +6746,10 @@
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C469" s="5" t="s">
         <v>5</v>
@@ -6757,10 +6766,10 @@
     </row>
     <row r="472" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>5</v>
@@ -6768,10 +6777,10 @@
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C473" s="5" t="s">
         <v>5</v>
@@ -6779,10 +6788,10 @@
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C474" s="5" t="s">
         <v>5</v>
@@ -6790,10 +6799,10 @@
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C475" s="5" t="s">
         <v>5</v>
@@ -6801,10 +6810,10 @@
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C476" s="5" t="s">
         <v>5</v>
@@ -6812,10 +6821,10 @@
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>5</v>
@@ -6823,10 +6832,10 @@
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>5</v>
@@ -6834,10 +6843,10 @@
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>5</v>
@@ -6845,10 +6854,10 @@
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>5</v>
@@ -6856,10 +6865,10 @@
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B481" s="13" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C481" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Adding next set of Stacks and Queues questions and Updating List.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="474">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1440,6 +1440,12 @@
   </si>
   <si>
     <t>Power Set</t>
+  </si>
+  <si>
+    <t>Stack or Two Pointers</t>
+  </si>
+  <si>
+    <t>Recursion ??</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1508,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1545,6 +1551,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1559,7 +1571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1625,6 +1637,16 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1977,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B294" sqref="B294"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A305" sqref="A305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -5192,106 +5214,112 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="21">
-      <c r="A305" s="12" t="s">
+    <row r="305" spans="1:4" ht="21">
+      <c r="A305" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B305" s="13" t="s">
+      <c r="B305" s="28" t="s">
         <v>303</v>
       </c>
-      <c r="C305" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" ht="21">
-      <c r="A306" s="12" t="s">
+      <c r="C305" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D305" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" ht="21">
+      <c r="A306" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B306" s="13" t="s">
+      <c r="B306" s="28" t="s">
         <v>304</v>
       </c>
-      <c r="C306" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" ht="21">
-      <c r="A307" s="12" t="s">
+      <c r="C306" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" ht="21">
+      <c r="A307" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B307" s="13" t="s">
+      <c r="B307" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="C307" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" ht="21">
-      <c r="A308" s="12" t="s">
+      <c r="C307" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" ht="21">
+      <c r="A308" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="B308" s="13" t="s">
+      <c r="B308" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="C308" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" ht="21">
-      <c r="A309" s="12" t="s">
+      <c r="C308" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D308" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" ht="21">
+      <c r="A309" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B309" s="26" t="s">
+      <c r="B309" s="33" t="s">
         <v>307</v>
       </c>
-      <c r="C309" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" ht="21">
-      <c r="A310" s="12" t="s">
+      <c r="C309" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" ht="21">
+      <c r="A310" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B310" s="13" t="s">
+      <c r="B310" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="C310" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" ht="21">
-      <c r="A311" s="12" t="s">
+      <c r="C310" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" ht="21">
+      <c r="A311" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B311" s="13" t="s">
+      <c r="B311" s="28" t="s">
         <v>309</v>
       </c>
-      <c r="C311" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" ht="21">
-      <c r="A312" s="12" t="s">
+      <c r="C311" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" ht="21">
+      <c r="A312" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B312" s="13" t="s">
+      <c r="B312" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="C312" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" ht="21">
-      <c r="A313" s="12" t="s">
+      <c r="C312" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" ht="21">
+      <c r="A313" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="B313" s="13" t="s">
+      <c r="B313" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="C313" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" ht="21">
+      <c r="C313" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" ht="21">
       <c r="A314" s="12" t="s">
         <v>293</v>
       </c>
@@ -5302,7 +5330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:3" ht="21">
+    <row r="315" spans="1:4" ht="21">
       <c r="A315" s="12" t="s">
         <v>293</v>
       </c>
@@ -5313,7 +5341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="316" spans="1:3" ht="21">
+    <row r="316" spans="1:4" ht="21">
       <c r="A316" s="12" t="s">
         <v>293</v>
       </c>
@@ -5324,7 +5352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:3" ht="21">
+    <row r="317" spans="1:4" ht="21">
       <c r="A317" s="12" t="s">
         <v>293</v>
       </c>
@@ -5335,7 +5363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="318" spans="1:3" ht="21">
+    <row r="318" spans="1:4" ht="21">
       <c r="A318" s="12" t="s">
         <v>293</v>
       </c>
@@ -5346,7 +5374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="319" spans="1:3" ht="21">
+    <row r="319" spans="1:4" ht="21">
       <c r="A319" s="12" t="s">
         <v>293</v>
       </c>
@@ -5357,7 +5385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="320" spans="1:3" ht="21">
+    <row r="320" spans="1:4" ht="21">
       <c r="A320" s="12" t="s">
         <v>293</v>
       </c>

</xml_diff>

<commit_message>
Adding next set of questions of Stacks and Queues and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -1532,7 +1532,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1542,7 +1542,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF224B12"/>
-        <bgColor rgb="FF395511"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
@@ -1554,7 +1554,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF127622"/>
-        <bgColor rgb="FF385724"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -1567,18 +1567,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF3FAF46"/>
         <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF385724"/>
-        <bgColor rgb="FF395511"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF395511"/>
-        <bgColor rgb="FF385724"/>
       </patternFill>
     </fill>
   </fills>
@@ -1619,7 +1607,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1724,34 +1712,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1818,12 +1778,12 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF3FAF46"/>
-      <rgbColor rgb="FF395511"/>
+      <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF224B12"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1836,11 +1796,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A319" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A325" activeCellId="0" sqref="A325"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B322" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B322" activeCellId="0" sqref="B322"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.63671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -4953,46 +4913,46 @@
       <c r="C295" s="5"/>
     </row>
     <row r="296" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B296" s="27" t="s">
+      <c r="B296" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="C296" s="28" t="s">
+      <c r="C296" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="26" t="s">
+      <c r="A297" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B297" s="27" t="s">
+      <c r="B297" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C297" s="28" t="s">
+      <c r="C297" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="26" t="s">
+      <c r="A298" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B298" s="27" t="s">
+      <c r="B298" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="C298" s="28" t="s">
+      <c r="C298" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="26" t="s">
+      <c r="A299" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B299" s="27" t="s">
+      <c r="B299" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C299" s="28" t="s">
+      <c r="C299" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5008,57 +4968,57 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="26" t="s">
+      <c r="A301" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B301" s="27" t="s">
+      <c r="B301" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C301" s="28" t="s">
+      <c r="C301" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="26" t="s">
+      <c r="A302" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B302" s="27" t="s">
+      <c r="B302" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C302" s="28" t="s">
+      <c r="C302" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="26" t="s">
+      <c r="A303" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B303" s="27" t="s">
+      <c r="B303" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="C303" s="28" t="s">
+      <c r="C303" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="26" t="s">
+      <c r="A304" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B304" s="27" t="s">
+      <c r="B304" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="C304" s="28" t="s">
+      <c r="C304" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="26" t="s">
+      <c r="A305" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B305" s="27" t="s">
+      <c r="B305" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="C305" s="28" t="s">
+      <c r="C305" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D305" s="0" t="s">
@@ -5066,24 +5026,24 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="26" t="s">
+      <c r="A306" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B306" s="27" t="s">
+      <c r="B306" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="C306" s="28" t="s">
+      <c r="C306" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="26" t="s">
+      <c r="A307" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B307" s="27" t="s">
+      <c r="B307" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="C307" s="28" t="s">
+      <c r="C307" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5102,112 +5062,112 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="26" t="s">
+      <c r="A309" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B309" s="29" t="s">
+      <c r="B309" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="C309" s="28" t="s">
+      <c r="C309" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="26" t="s">
+      <c r="A310" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B310" s="27" t="s">
+      <c r="B310" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="C310" s="28" t="s">
+      <c r="C310" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="26" t="s">
+      <c r="A311" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B311" s="27" t="s">
+      <c r="B311" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="C311" s="28" t="s">
+      <c r="C311" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="26" t="s">
+      <c r="A312" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B312" s="27" t="s">
+      <c r="B312" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C312" s="28" t="s">
+      <c r="C312" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="26" t="s">
+      <c r="A313" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B313" s="27" t="s">
+      <c r="B313" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C313" s="28" t="s">
+      <c r="C313" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="30" t="s">
+      <c r="A314" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B314" s="31" t="s">
+      <c r="B314" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="C314" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="30" t="s">
+      <c r="C314" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B315" s="31" t="s">
+      <c r="B315" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="C315" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="30" t="s">
+      <c r="C315" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B316" s="31" t="s">
+      <c r="B316" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="C316" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="30" t="s">
+      <c r="C316" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B317" s="31" t="s">
+      <c r="B317" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="C317" s="32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="30" t="s">
+      <c r="C317" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B318" s="31" t="s">
+      <c r="B318" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="C318" s="32" t="s">
+      <c r="C318" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5223,24 +5183,24 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="30" t="s">
+      <c r="A320" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B320" s="31" t="s">
+      <c r="B320" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="C320" s="32" t="s">
+      <c r="C320" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="30" t="s">
+      <c r="A321" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B321" s="31" t="s">
+      <c r="B321" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="C321" s="32" t="s">
+      <c r="C321" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D321" s="0" t="s">
@@ -5248,35 +5208,35 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="30" t="s">
+      <c r="A322" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B322" s="31" t="s">
+      <c r="B322" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C322" s="32" t="s">
+      <c r="C322" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="30" t="s">
+      <c r="A323" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B323" s="31" t="s">
+      <c r="B323" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="C323" s="32" t="s">
+      <c r="C323" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="30" t="s">
+      <c r="A324" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B324" s="31" t="s">
+      <c r="B324" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="C324" s="32" t="s">
+      <c r="C324" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D324" s="0" t="s">
@@ -5284,27 +5244,27 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="30" t="s">
+      <c r="A325" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B325" s="31" t="s">
+      <c r="B325" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="C325" s="32" t="s">
+      <c r="C325" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D325" s="0" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="12" t="s">
+    <row r="326" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B326" s="13" t="s">
+      <c r="B326" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="C326" s="5" t="s">
+      <c r="C326" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5320,68 +5280,68 @@
       </c>
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="12" t="s">
+      <c r="A328" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B328" s="13" t="s">
+      <c r="B328" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="C328" s="5" t="s">
+      <c r="C328" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="12" t="s">
+      <c r="A329" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B329" s="13" t="s">
+      <c r="B329" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="C329" s="5" t="s">
+      <c r="C329" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="12" t="s">
+      <c r="A330" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B330" s="13" t="s">
+      <c r="B330" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="C330" s="5" t="s">
+      <c r="C330" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="12" t="s">
+      <c r="A331" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B331" s="13" t="s">
+      <c r="B331" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="C331" s="5" t="s">
+      <c r="C331" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="12" t="s">
+      <c r="A332" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B332" s="13" t="s">
+      <c r="B332" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="C332" s="5" t="s">
+      <c r="C332" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="12" t="s">
+      <c r="A333" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B333" s="13" t="s">
+      <c r="B333" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="C333" s="5" t="s">
+      <c r="C333" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5485,7 +5445,7 @@
       <c r="A344" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="B344" s="33" t="s">
+      <c r="B344" s="26" t="s">
         <v>346</v>
       </c>
       <c r="C344" s="5" t="s">

</xml_diff>

<commit_message>
Adding heap questions and updating list.
</commit_message>
<xml_diff>
--- a/java/resources/FINAL450.xlsx
+++ b/java/resources/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="478">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -962,6 +962,9 @@
   </si>
   <si>
     <t xml:space="preserve">Length of the Longest Valid Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left, right</t>
   </si>
   <si>
     <t xml:space="preserve">Expression contains redundant bracket or not</t>
@@ -1532,7 +1535,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1554,7 +1557,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF127622"/>
-        <bgColor rgb="FF008080"/>
+        <bgColor rgb="FF069A2E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1566,7 +1569,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF3FAF46"/>
-        <bgColor rgb="FF33CCCC"/>
+        <bgColor rgb="FF069A2E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF069A2E"/>
+        <bgColor rgb="FF127622"/>
       </patternFill>
     </fill>
   </fills>
@@ -1607,7 +1616,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1712,6 +1721,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1741,7 +1754,7 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF069A2E"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
@@ -1796,11 +1809,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B322" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B322" activeCellId="0" sqref="B322"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A334" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B336" activeCellId="0" sqref="B336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3628,13 +3641,13 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="12" t="s">
+      <c r="A174" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B174" s="13" t="s">
+      <c r="B174" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C174" s="5" t="s">
+      <c r="C174" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5004,7 +5017,7 @@
       <c r="A304" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B304" s="7" t="s">
+      <c r="B304" s="26" t="s">
         <v>302</v>
       </c>
       <c r="C304" s="8" t="s">
@@ -5115,13 +5128,16 @@
       <c r="C313" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="D313" s="0" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="6" t="s">
         <v>293</v>
       </c>
       <c r="B314" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C314" s="8" t="s">
         <v>5</v>
@@ -5132,7 +5148,7 @@
         <v>293</v>
       </c>
       <c r="B315" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C315" s="8" t="s">
         <v>5</v>
@@ -5143,7 +5159,7 @@
         <v>293</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C316" s="8" t="s">
         <v>5</v>
@@ -5154,7 +5170,7 @@
         <v>293</v>
       </c>
       <c r="B317" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C317" s="8" t="s">
         <v>5</v>
@@ -5165,7 +5181,7 @@
         <v>293</v>
       </c>
       <c r="B318" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C318" s="8" t="s">
         <v>5</v>
@@ -5176,7 +5192,7 @@
         <v>293</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>5</v>
@@ -5187,7 +5203,7 @@
         <v>293</v>
       </c>
       <c r="B320" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C320" s="8" t="s">
         <v>5</v>
@@ -5197,14 +5213,14 @@
       <c r="A321" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B321" s="7" t="s">
-        <v>321</v>
+      <c r="B321" s="26" t="s">
+        <v>322</v>
       </c>
       <c r="C321" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5212,7 +5228,7 @@
         <v>293</v>
       </c>
       <c r="B322" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C322" s="8" t="s">
         <v>5</v>
@@ -5223,7 +5239,7 @@
         <v>293</v>
       </c>
       <c r="B323" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C323" s="8" t="s">
         <v>5</v>
@@ -5234,13 +5250,13 @@
         <v>293</v>
       </c>
       <c r="B324" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C324" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D324" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,13 +5264,13 @@
         <v>293</v>
       </c>
       <c r="B325" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C325" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D325" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5262,7 +5278,7 @@
         <v>293</v>
       </c>
       <c r="B326" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C326" s="8" t="s">
         <v>5</v>
@@ -5273,7 +5289,7 @@
         <v>293</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C327" s="5" t="s">
         <v>5</v>
@@ -5284,7 +5300,7 @@
         <v>293</v>
       </c>
       <c r="B328" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C328" s="8" t="s">
         <v>5</v>
@@ -5295,7 +5311,7 @@
         <v>293</v>
       </c>
       <c r="B329" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C329" s="8" t="s">
         <v>5</v>
@@ -5306,7 +5322,7 @@
         <v>293</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C330" s="8" t="s">
         <v>5</v>
@@ -5317,7 +5333,7 @@
         <v>293</v>
       </c>
       <c r="B331" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C331" s="8" t="s">
         <v>5</v>
@@ -5328,7 +5344,7 @@
         <v>293</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C332" s="8" t="s">
         <v>5</v>
@@ -5339,7 +5355,7 @@
         <v>293</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C333" s="8" t="s">
         <v>5</v>
@@ -5354,44 +5370,44 @@
       <c r="C335" s="5"/>
     </row>
     <row r="336" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B336" s="13" t="s">
+      <c r="A336" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C336" s="5" t="s">
+      <c r="B336" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C336" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B337" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="C337" s="5" t="s">
+      <c r="A337" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B337" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C337" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B338" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="C338" s="5" t="s">
+      <c r="A338" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B338" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C338" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>5</v>
@@ -5399,10 +5415,10 @@
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>5</v>
@@ -5410,10 +5426,10 @@
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>5</v>
@@ -5421,10 +5437,10 @@
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>5</v>
@@ -5432,10 +5448,10 @@
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C343" s="5" t="s">
         <v>5</v>
@@ -5443,10 +5459,10 @@
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B344" s="26" t="s">
-        <v>346</v>
+        <v>338</v>
+      </c>
+      <c r="B344" s="27" t="s">
+        <v>347</v>
       </c>
       <c r="C344" s="5" t="s">
         <v>5</v>
@@ -5454,10 +5470,10 @@
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>5</v>
@@ -5465,10 +5481,10 @@
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>5</v>
@@ -5476,10 +5492,10 @@
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>5</v>
@@ -5487,10 +5503,10 @@
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>5</v>
@@ -5498,10 +5514,10 @@
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>5</v>
@@ -5509,10 +5525,10 @@
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C350" s="5" t="s">
         <v>5</v>
@@ -5520,10 +5536,10 @@
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>5</v>
@@ -5531,10 +5547,10 @@
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>5</v>
@@ -5542,10 +5558,10 @@
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C353" s="5" t="s">
         <v>5</v>
@@ -5561,10 +5577,10 @@
     </row>
     <row r="356" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>5</v>
@@ -5572,10 +5588,10 @@
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C357" s="5" t="s">
         <v>5</v>
@@ -5583,10 +5599,10 @@
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>5</v>
@@ -5594,10 +5610,10 @@
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>5</v>
@@ -5605,10 +5621,10 @@
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C360" s="5" t="s">
         <v>5</v>
@@ -5616,10 +5632,10 @@
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C361" s="5" t="s">
         <v>5</v>
@@ -5627,10 +5643,10 @@
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C362" s="5" t="s">
         <v>5</v>
@@ -5638,10 +5654,10 @@
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>5</v>
@@ -5649,10 +5665,10 @@
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>5</v>
@@ -5660,10 +5676,10 @@
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>5</v>
@@ -5671,10 +5687,10 @@
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C366" s="5" t="s">
         <v>5</v>
@@ -5682,10 +5698,10 @@
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C367" s="5" t="s">
         <v>5</v>
@@ -5693,10 +5709,10 @@
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C368" s="5" t="s">
         <v>5</v>
@@ -5704,10 +5720,10 @@
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C369" s="5" t="s">
         <v>5</v>
@@ -5715,10 +5731,10 @@
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>5</v>
@@ -5726,10 +5742,10 @@
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C371" s="5" t="s">
         <v>5</v>
@@ -5737,10 +5753,10 @@
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C372" s="5" t="s">
         <v>5</v>
@@ -5748,10 +5764,10 @@
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C373" s="5" t="s">
         <v>5</v>
@@ -5759,10 +5775,10 @@
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>5</v>
@@ -5770,10 +5786,10 @@
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C375" s="5" t="s">
         <v>5</v>
@@ -5781,10 +5797,10 @@
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C376" s="5" t="s">
         <v>5</v>
@@ -5792,10 +5808,10 @@
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C377" s="5" t="s">
         <v>5</v>
@@ -5803,10 +5819,10 @@
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>5</v>
@@ -5814,10 +5830,10 @@
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C379" s="5" t="s">
         <v>5</v>
@@ -5825,10 +5841,10 @@
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C380" s="5" t="s">
         <v>5</v>
@@ -5836,10 +5852,10 @@
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C381" s="5" t="s">
         <v>5</v>
@@ -5847,10 +5863,10 @@
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C382" s="5" t="s">
         <v>5</v>
@@ -5858,10 +5874,10 @@
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C383" s="5" t="s">
         <v>5</v>
@@ -5869,10 +5885,10 @@
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C384" s="5" t="s">
         <v>5</v>
@@ -5880,10 +5896,10 @@
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>5</v>
@@ -5891,10 +5907,10 @@
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>5</v>
@@ -5902,10 +5918,10 @@
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>5</v>
@@ -5913,10 +5929,10 @@
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>5</v>
@@ -5924,10 +5940,10 @@
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>5</v>
@@ -5935,10 +5951,10 @@
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>5</v>
@@ -5946,10 +5962,10 @@
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>5</v>
@@ -5957,10 +5973,10 @@
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>5</v>
@@ -5968,10 +5984,10 @@
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>5</v>
@@ -5979,10 +5995,10 @@
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>5</v>
@@ -5990,10 +6006,10 @@
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>5</v>
@@ -6001,10 +6017,10 @@
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>5</v>
@@ -6012,10 +6028,10 @@
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>5</v>
@@ -6023,10 +6039,10 @@
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>5</v>
@@ -6034,10 +6050,10 @@
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C399" s="5" t="s">
         <v>5</v>
@@ -6053,10 +6069,10 @@
     </row>
     <row r="402" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>5</v>
@@ -6064,10 +6080,10 @@
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C403" s="5" t="s">
         <v>5</v>
@@ -6075,10 +6091,10 @@
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C404" s="5" t="s">
         <v>5</v>
@@ -6086,7 +6102,7 @@
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B405" s="13" t="s">
         <v>90</v>
@@ -6097,10 +6113,10 @@
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C406" s="5" t="s">
         <v>5</v>
@@ -6108,10 +6124,10 @@
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="12" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C407" s="5" t="s">
         <v>5</v>
@@ -6127,10 +6143,10 @@
     </row>
     <row r="410" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C410" s="5" t="s">
         <v>5</v>
@@ -6138,10 +6154,10 @@
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C411" s="5" t="s">
         <v>5</v>
@@ -6149,10 +6165,10 @@
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C412" s="5" t="s">
         <v>5</v>
@@ -6160,10 +6176,10 @@
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C413" s="5" t="s">
         <v>5</v>
@@ -6171,10 +6187,10 @@
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C414" s="5" t="s">
         <v>5</v>
@@ -6182,10 +6198,10 @@
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>5</v>
@@ -6193,10 +6209,10 @@
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C416" s="5" t="s">
         <v>5</v>
@@ -6204,7 +6220,7 @@
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B417" s="13" t="s">
         <v>281</v>
@@ -6215,10 +6231,10 @@
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C418" s="5" t="s">
         <v>5</v>
@@ -6226,10 +6242,10 @@
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C419" s="5" t="s">
         <v>5</v>
@@ -6237,10 +6253,10 @@
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C420" s="5" t="s">
         <v>5</v>
@@ -6248,10 +6264,10 @@
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C421" s="5" t="s">
         <v>5</v>
@@ -6259,10 +6275,10 @@
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>5</v>
@@ -6270,10 +6286,10 @@
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C423" s="5" t="s">
         <v>5</v>
@@ -6281,10 +6297,10 @@
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C424" s="5" t="s">
         <v>5</v>
@@ -6292,10 +6308,10 @@
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C425" s="5" t="s">
         <v>5</v>
@@ -6303,10 +6319,10 @@
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C426" s="5" t="s">
         <v>5</v>
@@ -6314,10 +6330,10 @@
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C427" s="5" t="s">
         <v>5</v>
@@ -6325,10 +6341,10 @@
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C428" s="5" t="s">
         <v>5</v>
@@ -6336,10 +6352,10 @@
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>5</v>
@@ -6347,10 +6363,10 @@
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>5</v>
@@ -6358,10 +6374,10 @@
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C431" s="5" t="s">
         <v>5</v>
@@ -6369,10 +6385,10 @@
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C432" s="5" t="s">
         <v>5</v>
@@ -6380,10 +6396,10 @@
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C433" s="5" t="s">
         <v>5</v>
@@ -6391,10 +6407,10 @@
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C434" s="5" t="s">
         <v>5</v>
@@ -6402,10 +6418,10 @@
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C435" s="5" t="s">
         <v>5</v>
@@ -6413,10 +6429,10 @@
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C436" s="5" t="s">
         <v>5</v>
@@ -6424,10 +6440,10 @@
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>5</v>
@@ -6435,10 +6451,10 @@
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C438" s="5" t="s">
         <v>5</v>
@@ -6446,10 +6462,10 @@
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>5</v>
@@ -6457,10 +6473,10 @@
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C440" s="5" t="s">
         <v>5</v>
@@ -6468,10 +6484,10 @@
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C441" s="5" t="s">
         <v>5</v>
@@ -6479,10 +6495,10 @@
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>5</v>
@@ -6490,10 +6506,10 @@
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>5</v>
@@ -6501,10 +6517,10 @@
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>5</v>
@@ -6512,10 +6528,10 @@
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>5</v>
@@ -6523,10 +6539,10 @@
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>5</v>
@@ -6534,10 +6550,10 @@
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C447" s="5" t="s">
         <v>5</v>
@@ -6545,10 +6561,10 @@
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>5</v>
@@ -6556,10 +6572,10 @@
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C449" s="5" t="s">
         <v>5</v>
@@ -6567,10 +6583,10 @@
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C450" s="5" t="s">
         <v>5</v>
@@ -6578,10 +6594,10 @@
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>5</v>
@@ -6589,10 +6605,10 @@
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>5</v>
@@ -6600,10 +6616,10 @@
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>5</v>
@@ -6611,10 +6627,10 @@
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>5</v>
@@ -6622,10 +6638,10 @@
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C455" s="5" t="s">
         <v>5</v>
@@ -6633,10 +6649,10 @@
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C456" s="5" t="s">
         <v>5</v>
@@ -6644,10 +6660,10 @@
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C457" s="5" t="s">
         <v>5</v>
@@ -6655,10 +6671,10 @@
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C458" s="5" t="s">
         <v>5</v>
@@ -6666,10 +6682,10 @@
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C459" s="5" t="s">
         <v>5</v>
@@ -6677,10 +6693,10 @@
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>5</v>
@@ -6688,10 +6704,10 @@
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>5</v>
@@ -6699,10 +6715,10 @@
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>5</v>
@@ -6710,10 +6726,10 @@
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>5</v>
@@ -6721,10 +6737,10 @@
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>5</v>
@@ -6732,10 +6748,10 @@
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C465" s="5" t="s">
         <v>5</v>
@@ -6743,10 +6759,10 @@
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>5</v>
@@ -6754,10 +6770,10 @@
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C467" s="5" t="s">
         <v>5</v>
@@ -6765,10 +6781,10 @@
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>5</v>
@@ -6776,10 +6792,10 @@
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C469" s="5" t="s">
         <v>5</v>
@@ -6796,10 +6812,10 @@
     </row>
     <row r="472" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>5</v>
@@ -6807,10 +6823,10 @@
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C473" s="5" t="s">
         <v>5</v>
@@ -6818,10 +6834,10 @@
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C474" s="5" t="s">
         <v>5</v>
@@ -6829,10 +6845,10 @@
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C475" s="5" t="s">
         <v>5</v>
@@ -6840,10 +6856,10 @@
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C476" s="5" t="s">
         <v>5</v>
@@ -6851,10 +6867,10 @@
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>5</v>
@@ -6862,10 +6878,10 @@
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>5</v>
@@ -6873,10 +6889,10 @@
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>5</v>
@@ -6884,10 +6900,10 @@
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>5</v>
@@ -6895,10 +6911,10 @@
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="12" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B481" s="13" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C481" s="5" t="s">
         <v>5</v>

</xml_diff>